<commit_message>
add adult_total to excel upload logic
</commit_message>
<xml_diff>
--- a/django_project/frontend/tests/csv/excel_error_property.xlsx
+++ b/django_project/frontend/tests/csv/excel_error_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Impt Backup\sanbi\test_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3599134-8E3F-4EEE-AC20-08F29AF1AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2CAC7A-93CC-4E88-916F-C31C82D412C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="4155" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,11 @@
     <sheet name="Scientific name dropdown" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7142" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="622">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1918,6 +1917,9 @@
   </si>
   <si>
     <t>Property_code</t>
+  </si>
+  <si>
+    <t>COUNT_adult_TOTAL</t>
   </si>
 </sst>
 </file>
@@ -24334,10 +24336,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BH95"/>
+  <dimension ref="A1:BI95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24346,15 +24348,22 @@
     <col min="2" max="2" width="15.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
     <col min="4" max="6" width="21.7109375" style="4" customWidth="1"/>
-    <col min="7" max="18" width="8.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" style="4" customWidth="1"/>
-    <col min="20" max="21" width="8.42578125" style="4" customWidth="1"/>
-    <col min="22" max="23" width="30.28515625" style="4" customWidth="1"/>
-    <col min="24" max="61" width="8.42578125" style="4" customWidth="1"/>
-    <col min="62" max="16384" width="8.42578125" style="4"/>
+    <col min="7" max="7" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="8.42578125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="40.85546875" style="4" customWidth="1"/>
+    <col min="21" max="22" width="8.42578125" style="4" customWidth="1"/>
+    <col min="23" max="24" width="30.28515625" style="4" customWidth="1"/>
+    <col min="25" max="62" width="8.42578125" style="4" customWidth="1"/>
+    <col min="63" max="16384" width="8.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="87" t="s">
         <v>620</v>
       </c>
@@ -24377,166 +24386,169 @@
         <v>32</v>
       </c>
       <c r="H1" s="94" t="s">
+        <v>621</v>
+      </c>
+      <c r="I1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="J1" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="L1" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="M1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="N1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="O1" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="P1" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="Q1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="93" t="s">
+      <c r="R1" s="93" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="95" t="s">
+      <c r="S1" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="T1" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="93" t="s">
+      <c r="U1" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="95" t="s">
+      <c r="V1" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="93" t="s">
+      <c r="W1" s="93" t="s">
         <v>143</v>
       </c>
-      <c r="W1" s="95" t="s">
+      <c r="X1" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="93" t="s">
+      <c r="Y1" s="93" t="s">
         <v>144</v>
       </c>
-      <c r="Y1" s="96" t="s">
+      <c r="Z1" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" s="62" t="s">
+      <c r="AA1" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" s="63" t="s">
+      <c r="AB1" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AC1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="63" t="s">
+      <c r="AD1" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="63" t="s">
+      <c r="AE1" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="63" t="s">
+      <c r="AF1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" s="63" t="s">
+      <c r="AG1" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="62" t="s">
+      <c r="AH1" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="AH1" s="62" t="s">
+      <c r="AI1" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="64" t="s">
+      <c r="AJ1" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="97" t="s">
+      <c r="AK1" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="AK1" s="98" t="s">
+      <c r="AL1" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="AL1" s="63" t="s">
+      <c r="AM1" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" s="63" t="s">
+      <c r="AN1" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="AN1" s="63" t="s">
+      <c r="AO1" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AO1" s="63" t="s">
+      <c r="AP1" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" s="62" t="s">
+      <c r="AQ1" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="AQ1" s="62" t="s">
+      <c r="AR1" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="AR1" s="62" t="s">
+      <c r="AS1" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="AS1" s="63" t="s">
+      <c r="AT1" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AT1" s="63" t="s">
+      <c r="AU1" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="AU1" s="63" t="s">
+      <c r="AV1" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="AV1" s="63" t="s">
+      <c r="AW1" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AW1" s="62" t="s">
+      <c r="AX1" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="AX1" s="62" t="s">
+      <c r="AY1" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AY1" s="63" t="s">
+      <c r="AZ1" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" s="63" t="s">
+      <c r="BA1" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="BA1" s="63" t="s">
+      <c r="BB1" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="BB1" s="63" t="s">
+      <c r="BC1" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="BC1" s="62" t="s">
+      <c r="BD1" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="BD1" s="62" t="s">
+      <c r="BE1" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="BE1" s="63" t="s">
+      <c r="BF1" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="BF1" s="63" t="s">
+      <c r="BG1" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="BG1" s="63" t="s">
+      <c r="BH1" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="BH1" s="67" t="s">
+      <c r="BI1" s="67" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>179</v>
       </c>
@@ -24556,66 +24568,68 @@
         <v>2021</v>
       </c>
       <c r="G2" s="23">
-        <f>SUM(H2:I2,J2,M2)</f>
+        <f>SUM(I2:J2,K2,N2)</f>
         <v>357</v>
       </c>
       <c r="H2" s="23">
+        <v>268</v>
+      </c>
+      <c r="I2" s="23">
         <v>145</v>
       </c>
-      <c r="I2" s="23">
+      <c r="J2" s="23">
         <v>123</v>
       </c>
-      <c r="J2" s="23">
+      <c r="K2" s="23">
         <v>55</v>
       </c>
-      <c r="K2" s="23">
+      <c r="L2" s="23">
         <v>35</v>
       </c>
-      <c r="L2" s="23">
+      <c r="M2" s="23">
         <v>20</v>
       </c>
-      <c r="M2" s="23">
+      <c r="N2" s="23">
         <v>34</v>
       </c>
-      <c r="N2" s="23">
+      <c r="O2" s="23">
         <v>22</v>
       </c>
-      <c r="O2" s="23">
+      <c r="P2" s="23">
         <v>12</v>
       </c>
-      <c r="P2" s="23">
+      <c r="Q2" s="23">
         <v>8</v>
       </c>
-      <c r="Q2" s="23">
+      <c r="R2" s="23">
         <v>53</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="T2" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="23"/>
-      <c r="U2" s="22" t="s">
+      <c r="U2" s="23"/>
+      <c r="V2" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="V2" s="23"/>
-      <c r="W2" s="22" t="s">
+      <c r="W2" s="23"/>
+      <c r="X2" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="X2" s="23">
+      <c r="Y2" s="23">
         <v>2</v>
       </c>
-      <c r="Y2" s="23">
+      <c r="Z2" s="23">
         <v>600</v>
       </c>
-      <c r="Z2" s="23">
+      <c r="AA2" s="23">
         <v>100</v>
       </c>
-      <c r="AA2" s="23">
+      <c r="AB2" s="23">
         <v>30</v>
       </c>
-      <c r="AB2" s="74"/>
       <c r="AC2" s="74"/>
       <c r="AD2" s="74"/>
       <c r="AE2" s="74"/>
@@ -24624,46 +24638,46 @@
       <c r="AH2" s="74"/>
       <c r="AI2" s="74"/>
       <c r="AJ2" s="74"/>
-      <c r="AK2" s="23">
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="23">
         <v>15</v>
-      </c>
-      <c r="AL2" s="23">
-        <v>7</v>
       </c>
       <c r="AM2" s="23">
         <v>7</v>
       </c>
       <c r="AN2" s="23">
+        <v>7</v>
+      </c>
+      <c r="AO2" s="23">
         <v>1</v>
       </c>
-      <c r="AO2" s="23">
+      <c r="AP2" s="23">
         <v>0</v>
       </c>
-      <c r="AP2" s="22" t="s">
+      <c r="AQ2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="AQ2" s="22" t="s">
+      <c r="AR2" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="AR2" s="23">
+      <c r="AS2" s="23">
         <v>22</v>
       </c>
-      <c r="AS2" s="23">
+      <c r="AT2" s="23">
         <v>10</v>
       </c>
-      <c r="AT2" s="23">
+      <c r="AU2" s="23">
         <v>2</v>
-      </c>
-      <c r="AU2" s="23">
-        <v>5</v>
       </c>
       <c r="AV2" s="23">
         <v>5</v>
       </c>
-      <c r="AW2" s="22" t="s">
+      <c r="AW2" s="23">
+        <v>5</v>
+      </c>
+      <c r="AX2" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="AX2" s="74"/>
       <c r="AY2" s="74"/>
       <c r="AZ2" s="74"/>
       <c r="BA2" s="74"/>
@@ -24674,8 +24688,9 @@
       <c r="BF2" s="74"/>
       <c r="BG2" s="74"/>
       <c r="BH2" s="74"/>
-    </row>
-    <row r="3" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI2" s="74"/>
+    </row>
+    <row r="3" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
       <c r="C3" s="22"/>
@@ -24695,10 +24710,10 @@
       <c r="Q3" s="74"/>
       <c r="R3" s="74"/>
       <c r="S3" s="74"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="23"/>
       <c r="X3" s="74"/>
       <c r="Y3" s="74"/>
       <c r="Z3" s="74"/>
@@ -24736,8 +24751,9 @@
       <c r="BF3" s="74"/>
       <c r="BG3" s="74"/>
       <c r="BH3" s="74"/>
-    </row>
-    <row r="4" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI3" s="74"/>
+    </row>
+    <row r="4" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74"/>
       <c r="B4" s="74"/>
       <c r="C4" s="22"/>
@@ -24757,10 +24773,10 @@
       <c r="Q4" s="74"/>
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="23"/>
       <c r="X4" s="74"/>
       <c r="Y4" s="74"/>
       <c r="Z4" s="74"/>
@@ -24798,8 +24814,9 @@
       <c r="BF4" s="74"/>
       <c r="BG4" s="74"/>
       <c r="BH4" s="74"/>
-    </row>
-    <row r="5" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="74"/>
+    </row>
+    <row r="5" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
       <c r="B5" s="74"/>
       <c r="C5" s="22"/>
@@ -24819,10 +24836,10 @@
       <c r="Q5" s="74"/>
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="23"/>
       <c r="X5" s="74"/>
       <c r="Y5" s="74"/>
       <c r="Z5" s="74"/>
@@ -24860,8 +24877,9 @@
       <c r="BF5" s="74"/>
       <c r="BG5" s="74"/>
       <c r="BH5" s="74"/>
-    </row>
-    <row r="6" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI5" s="74"/>
+    </row>
+    <row r="6" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="74"/>
       <c r="B6" s="74"/>
       <c r="C6" s="22"/>
@@ -24881,10 +24899,10 @@
       <c r="Q6" s="74"/>
       <c r="R6" s="74"/>
       <c r="S6" s="74"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="23"/>
       <c r="X6" s="74"/>
       <c r="Y6" s="74"/>
       <c r="Z6" s="74"/>
@@ -24922,8 +24940,9 @@
       <c r="BF6" s="74"/>
       <c r="BG6" s="74"/>
       <c r="BH6" s="74"/>
-    </row>
-    <row r="7" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI6" s="74"/>
+    </row>
+    <row r="7" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74"/>
       <c r="B7" s="74"/>
       <c r="C7" s="22"/>
@@ -24943,10 +24962,10 @@
       <c r="Q7" s="74"/>
       <c r="R7" s="74"/>
       <c r="S7" s="74"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="23"/>
       <c r="X7" s="74"/>
       <c r="Y7" s="74"/>
       <c r="Z7" s="74"/>
@@ -24984,8 +25003,9 @@
       <c r="BF7" s="74"/>
       <c r="BG7" s="74"/>
       <c r="BH7" s="74"/>
-    </row>
-    <row r="8" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI7" s="74"/>
+    </row>
+    <row r="8" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74"/>
       <c r="B8" s="74"/>
       <c r="C8" s="22"/>
@@ -25005,10 +25025,10 @@
       <c r="Q8" s="74"/>
       <c r="R8" s="74"/>
       <c r="S8" s="74"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="23"/>
       <c r="X8" s="74"/>
       <c r="Y8" s="74"/>
       <c r="Z8" s="74"/>
@@ -25046,8 +25066,9 @@
       <c r="BF8" s="74"/>
       <c r="BG8" s="74"/>
       <c r="BH8" s="74"/>
-    </row>
-    <row r="9" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI8" s="74"/>
+    </row>
+    <row r="9" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74"/>
       <c r="B9" s="74"/>
       <c r="C9" s="22"/>
@@ -25067,10 +25088,10 @@
       <c r="Q9" s="74"/>
       <c r="R9" s="74"/>
       <c r="S9" s="74"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="23"/>
       <c r="X9" s="74"/>
       <c r="Y9" s="74"/>
       <c r="Z9" s="74"/>
@@ -25108,8 +25129,9 @@
       <c r="BF9" s="74"/>
       <c r="BG9" s="74"/>
       <c r="BH9" s="74"/>
-    </row>
-    <row r="10" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI9" s="74"/>
+    </row>
+    <row r="10" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74"/>
       <c r="B10" s="74"/>
       <c r="C10" s="22"/>
@@ -25129,10 +25151,10 @@
       <c r="Q10" s="74"/>
       <c r="R10" s="74"/>
       <c r="S10" s="74"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="23"/>
       <c r="X10" s="74"/>
       <c r="Y10" s="74"/>
       <c r="Z10" s="74"/>
@@ -25170,8 +25192,9 @@
       <c r="BF10" s="74"/>
       <c r="BG10" s="74"/>
       <c r="BH10" s="74"/>
-    </row>
-    <row r="11" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI10" s="74"/>
+    </row>
+    <row r="11" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="74"/>
       <c r="B11" s="74"/>
       <c r="C11" s="22"/>
@@ -25191,10 +25214,10 @@
       <c r="Q11" s="74"/>
       <c r="R11" s="74"/>
       <c r="S11" s="74"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="23"/>
       <c r="X11" s="74"/>
       <c r="Y11" s="74"/>
       <c r="Z11" s="74"/>
@@ -25232,8 +25255,9 @@
       <c r="BF11" s="74"/>
       <c r="BG11" s="74"/>
       <c r="BH11" s="74"/>
-    </row>
-    <row r="12" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI11" s="74"/>
+    </row>
+    <row r="12" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74"/>
       <c r="B12" s="74"/>
       <c r="C12" s="22"/>
@@ -25253,10 +25277,10 @@
       <c r="Q12" s="74"/>
       <c r="R12" s="74"/>
       <c r="S12" s="74"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="23"/>
       <c r="X12" s="74"/>
       <c r="Y12" s="74"/>
       <c r="Z12" s="74"/>
@@ -25294,8 +25318,9 @@
       <c r="BF12" s="74"/>
       <c r="BG12" s="74"/>
       <c r="BH12" s="74"/>
-    </row>
-    <row r="13" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI12" s="74"/>
+    </row>
+    <row r="13" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
       <c r="B13" s="74"/>
       <c r="C13" s="22"/>
@@ -25315,10 +25340,10 @@
       <c r="Q13" s="74"/>
       <c r="R13" s="74"/>
       <c r="S13" s="74"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="23"/>
       <c r="X13" s="74"/>
       <c r="Y13" s="74"/>
       <c r="Z13" s="74"/>
@@ -25356,8 +25381,9 @@
       <c r="BF13" s="74"/>
       <c r="BG13" s="74"/>
       <c r="BH13" s="74"/>
-    </row>
-    <row r="14" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI13" s="74"/>
+    </row>
+    <row r="14" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="74"/>
       <c r="C14" s="22"/>
@@ -25377,10 +25403,10 @@
       <c r="Q14" s="74"/>
       <c r="R14" s="74"/>
       <c r="S14" s="74"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="23"/>
       <c r="X14" s="74"/>
       <c r="Y14" s="74"/>
       <c r="Z14" s="74"/>
@@ -25418,8 +25444,9 @@
       <c r="BF14" s="74"/>
       <c r="BG14" s="74"/>
       <c r="BH14" s="74"/>
-    </row>
-    <row r="15" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI14" s="74"/>
+    </row>
+    <row r="15" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="74"/>
       <c r="C15" s="22"/>
@@ -25439,10 +25466,10 @@
       <c r="Q15" s="74"/>
       <c r="R15" s="74"/>
       <c r="S15" s="74"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="23"/>
       <c r="X15" s="74"/>
       <c r="Y15" s="74"/>
       <c r="Z15" s="74"/>
@@ -25480,8 +25507,9 @@
       <c r="BF15" s="74"/>
       <c r="BG15" s="74"/>
       <c r="BH15" s="74"/>
-    </row>
-    <row r="16" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI15" s="74"/>
+    </row>
+    <row r="16" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="74"/>
       <c r="C16" s="22"/>
@@ -25501,10 +25529,10 @@
       <c r="Q16" s="74"/>
       <c r="R16" s="74"/>
       <c r="S16" s="74"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="23"/>
       <c r="X16" s="74"/>
       <c r="Y16" s="74"/>
       <c r="Z16" s="74"/>
@@ -25542,8 +25570,9 @@
       <c r="BF16" s="74"/>
       <c r="BG16" s="74"/>
       <c r="BH16" s="74"/>
-    </row>
-    <row r="17" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI16" s="74"/>
+    </row>
+    <row r="17" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
       <c r="B17" s="74"/>
       <c r="C17" s="22"/>
@@ -25563,10 +25592,10 @@
       <c r="Q17" s="74"/>
       <c r="R17" s="74"/>
       <c r="S17" s="74"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="23"/>
       <c r="X17" s="74"/>
       <c r="Y17" s="74"/>
       <c r="Z17" s="74"/>
@@ -25604,8 +25633,9 @@
       <c r="BF17" s="74"/>
       <c r="BG17" s="74"/>
       <c r="BH17" s="74"/>
-    </row>
-    <row r="18" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI17" s="74"/>
+    </row>
+    <row r="18" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="74"/>
       <c r="C18" s="22"/>
@@ -25625,10 +25655,10 @@
       <c r="Q18" s="74"/>
       <c r="R18" s="74"/>
       <c r="S18" s="74"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="74"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="23"/>
       <c r="X18" s="74"/>
       <c r="Y18" s="74"/>
       <c r="Z18" s="74"/>
@@ -25666,8 +25696,9 @@
       <c r="BF18" s="74"/>
       <c r="BG18" s="74"/>
       <c r="BH18" s="74"/>
-    </row>
-    <row r="19" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI18" s="74"/>
+    </row>
+    <row r="19" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
       <c r="B19" s="74"/>
       <c r="C19" s="22"/>
@@ -25687,10 +25718,10 @@
       <c r="Q19" s="74"/>
       <c r="R19" s="74"/>
       <c r="S19" s="74"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="23"/>
       <c r="X19" s="74"/>
       <c r="Y19" s="74"/>
       <c r="Z19" s="74"/>
@@ -25728,8 +25759,9 @@
       <c r="BF19" s="74"/>
       <c r="BG19" s="74"/>
       <c r="BH19" s="74"/>
-    </row>
-    <row r="20" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI19" s="74"/>
+    </row>
+    <row r="20" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
       <c r="B20" s="74"/>
       <c r="C20" s="22"/>
@@ -25749,10 +25781,10 @@
       <c r="Q20" s="74"/>
       <c r="R20" s="74"/>
       <c r="S20" s="74"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="74"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="23"/>
       <c r="X20" s="74"/>
       <c r="Y20" s="74"/>
       <c r="Z20" s="74"/>
@@ -25790,8 +25822,9 @@
       <c r="BF20" s="74"/>
       <c r="BG20" s="74"/>
       <c r="BH20" s="74"/>
-    </row>
-    <row r="21" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI20" s="74"/>
+    </row>
+    <row r="21" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="74"/>
       <c r="C21" s="22"/>
@@ -25811,10 +25844,10 @@
       <c r="Q21" s="74"/>
       <c r="R21" s="74"/>
       <c r="S21" s="74"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="74"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="74"/>
+      <c r="T21" s="74"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="23"/>
       <c r="X21" s="74"/>
       <c r="Y21" s="74"/>
       <c r="Z21" s="74"/>
@@ -25852,8 +25885,9 @@
       <c r="BF21" s="74"/>
       <c r="BG21" s="74"/>
       <c r="BH21" s="74"/>
-    </row>
-    <row r="22" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI21" s="74"/>
+    </row>
+    <row r="22" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74"/>
       <c r="B22" s="74"/>
       <c r="C22" s="22"/>
@@ -25873,10 +25907,10 @@
       <c r="Q22" s="74"/>
       <c r="R22" s="74"/>
       <c r="S22" s="74"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="23"/>
       <c r="X22" s="74"/>
       <c r="Y22" s="74"/>
       <c r="Z22" s="74"/>
@@ -25914,8 +25948,9 @@
       <c r="BF22" s="74"/>
       <c r="BG22" s="74"/>
       <c r="BH22" s="74"/>
-    </row>
-    <row r="23" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI22" s="74"/>
+    </row>
+    <row r="23" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="74"/>
       <c r="B23" s="74"/>
       <c r="C23" s="22"/>
@@ -25935,10 +25970,10 @@
       <c r="Q23" s="74"/>
       <c r="R23" s="74"/>
       <c r="S23" s="74"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="74"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="23"/>
       <c r="X23" s="74"/>
       <c r="Y23" s="74"/>
       <c r="Z23" s="74"/>
@@ -25976,8 +26011,9 @@
       <c r="BF23" s="74"/>
       <c r="BG23" s="74"/>
       <c r="BH23" s="74"/>
-    </row>
-    <row r="24" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI23" s="74"/>
+    </row>
+    <row r="24" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="74"/>
       <c r="B24" s="74"/>
       <c r="C24" s="22"/>
@@ -25997,10 +26033,10 @@
       <c r="Q24" s="74"/>
       <c r="R24" s="74"/>
       <c r="S24" s="74"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="74"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="74"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="23"/>
       <c r="X24" s="74"/>
       <c r="Y24" s="74"/>
       <c r="Z24" s="74"/>
@@ -26038,8 +26074,9 @@
       <c r="BF24" s="74"/>
       <c r="BG24" s="74"/>
       <c r="BH24" s="74"/>
-    </row>
-    <row r="25" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI24" s="74"/>
+    </row>
+    <row r="25" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="74"/>
       <c r="B25" s="74"/>
       <c r="C25" s="22"/>
@@ -26059,10 +26096,10 @@
       <c r="Q25" s="74"/>
       <c r="R25" s="74"/>
       <c r="S25" s="74"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="23"/>
       <c r="X25" s="74"/>
       <c r="Y25" s="74"/>
       <c r="Z25" s="74"/>
@@ -26100,8 +26137,9 @@
       <c r="BF25" s="74"/>
       <c r="BG25" s="74"/>
       <c r="BH25" s="74"/>
-    </row>
-    <row r="26" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI25" s="74"/>
+    </row>
+    <row r="26" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="74"/>
       <c r="B26" s="74"/>
       <c r="C26" s="22"/>
@@ -26121,10 +26159,10 @@
       <c r="Q26" s="74"/>
       <c r="R26" s="74"/>
       <c r="S26" s="74"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="74"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="23"/>
       <c r="X26" s="74"/>
       <c r="Y26" s="74"/>
       <c r="Z26" s="74"/>
@@ -26162,8 +26200,9 @@
       <c r="BF26" s="74"/>
       <c r="BG26" s="74"/>
       <c r="BH26" s="74"/>
-    </row>
-    <row r="27" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI26" s="74"/>
+    </row>
+    <row r="27" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="74"/>
       <c r="B27" s="74"/>
       <c r="C27" s="22"/>
@@ -26183,10 +26222,10 @@
       <c r="Q27" s="74"/>
       <c r="R27" s="74"/>
       <c r="S27" s="74"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="74"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="74"/>
+      <c r="T27" s="74"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="23"/>
       <c r="X27" s="74"/>
       <c r="Y27" s="74"/>
       <c r="Z27" s="74"/>
@@ -26224,8 +26263,9 @@
       <c r="BF27" s="74"/>
       <c r="BG27" s="74"/>
       <c r="BH27" s="74"/>
-    </row>
-    <row r="28" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI27" s="74"/>
+    </row>
+    <row r="28" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="74"/>
       <c r="B28" s="74"/>
       <c r="C28" s="22"/>
@@ -26245,10 +26285,10 @@
       <c r="Q28" s="74"/>
       <c r="R28" s="74"/>
       <c r="S28" s="74"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="74"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="74"/>
+      <c r="T28" s="74"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="23"/>
       <c r="X28" s="74"/>
       <c r="Y28" s="74"/>
       <c r="Z28" s="74"/>
@@ -26286,8 +26326,9 @@
       <c r="BF28" s="74"/>
       <c r="BG28" s="74"/>
       <c r="BH28" s="74"/>
-    </row>
-    <row r="29" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI28" s="74"/>
+    </row>
+    <row r="29" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="74"/>
       <c r="B29" s="74"/>
       <c r="C29" s="22"/>
@@ -26307,10 +26348,10 @@
       <c r="Q29" s="74"/>
       <c r="R29" s="74"/>
       <c r="S29" s="74"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="74"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="23"/>
       <c r="X29" s="74"/>
       <c r="Y29" s="74"/>
       <c r="Z29" s="74"/>
@@ -26348,8 +26389,9 @@
       <c r="BF29" s="74"/>
       <c r="BG29" s="74"/>
       <c r="BH29" s="74"/>
-    </row>
-    <row r="30" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI29" s="74"/>
+    </row>
+    <row r="30" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74"/>
       <c r="B30" s="74"/>
       <c r="C30" s="22"/>
@@ -26369,10 +26411,10 @@
       <c r="Q30" s="74"/>
       <c r="R30" s="74"/>
       <c r="S30" s="74"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="74"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="74"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="23"/>
       <c r="X30" s="74"/>
       <c r="Y30" s="74"/>
       <c r="Z30" s="74"/>
@@ -26410,8 +26452,9 @@
       <c r="BF30" s="74"/>
       <c r="BG30" s="74"/>
       <c r="BH30" s="74"/>
-    </row>
-    <row r="31" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI30" s="74"/>
+    </row>
+    <row r="31" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74"/>
       <c r="B31" s="74"/>
       <c r="C31" s="22"/>
@@ -26431,10 +26474,10 @@
       <c r="Q31" s="74"/>
       <c r="R31" s="74"/>
       <c r="S31" s="74"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="74"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="74"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="23"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="23"/>
       <c r="X31" s="74"/>
       <c r="Y31" s="74"/>
       <c r="Z31" s="74"/>
@@ -26472,8 +26515,9 @@
       <c r="BF31" s="74"/>
       <c r="BG31" s="74"/>
       <c r="BH31" s="74"/>
-    </row>
-    <row r="32" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI31" s="74"/>
+    </row>
+    <row r="32" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="74"/>
       <c r="B32" s="74"/>
       <c r="C32" s="22"/>
@@ -26493,10 +26537,10 @@
       <c r="Q32" s="74"/>
       <c r="R32" s="74"/>
       <c r="S32" s="74"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="74"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="74"/>
+      <c r="T32" s="74"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="23"/>
       <c r="X32" s="74"/>
       <c r="Y32" s="74"/>
       <c r="Z32" s="74"/>
@@ -26534,8 +26578,9 @@
       <c r="BF32" s="74"/>
       <c r="BG32" s="74"/>
       <c r="BH32" s="74"/>
-    </row>
-    <row r="33" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI32" s="74"/>
+    </row>
+    <row r="33" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="74"/>
       <c r="B33" s="74"/>
       <c r="C33" s="22"/>
@@ -26555,10 +26600,10 @@
       <c r="Q33" s="74"/>
       <c r="R33" s="74"/>
       <c r="S33" s="74"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="74"/>
+      <c r="T33" s="74"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="23"/>
       <c r="X33" s="74"/>
       <c r="Y33" s="74"/>
       <c r="Z33" s="74"/>
@@ -26596,8 +26641,9 @@
       <c r="BF33" s="74"/>
       <c r="BG33" s="74"/>
       <c r="BH33" s="74"/>
-    </row>
-    <row r="34" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI33" s="74"/>
+    </row>
+    <row r="34" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74"/>
       <c r="B34" s="74"/>
       <c r="C34" s="22"/>
@@ -26617,10 +26663,10 @@
       <c r="Q34" s="74"/>
       <c r="R34" s="74"/>
       <c r="S34" s="74"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="74"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="23"/>
       <c r="X34" s="74"/>
       <c r="Y34" s="74"/>
       <c r="Z34" s="74"/>
@@ -26658,8 +26704,9 @@
       <c r="BF34" s="74"/>
       <c r="BG34" s="74"/>
       <c r="BH34" s="74"/>
-    </row>
-    <row r="35" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI34" s="74"/>
+    </row>
+    <row r="35" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="74"/>
       <c r="B35" s="74"/>
       <c r="C35" s="22"/>
@@ -26679,10 +26726,10 @@
       <c r="Q35" s="74"/>
       <c r="R35" s="74"/>
       <c r="S35" s="74"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="74"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="74"/>
+      <c r="T35" s="74"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="23"/>
       <c r="X35" s="74"/>
       <c r="Y35" s="74"/>
       <c r="Z35" s="74"/>
@@ -26720,8 +26767,9 @@
       <c r="BF35" s="74"/>
       <c r="BG35" s="74"/>
       <c r="BH35" s="74"/>
-    </row>
-    <row r="36" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI35" s="74"/>
+    </row>
+    <row r="36" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="74"/>
       <c r="B36" s="74"/>
       <c r="C36" s="22"/>
@@ -26741,10 +26789,10 @@
       <c r="Q36" s="74"/>
       <c r="R36" s="74"/>
       <c r="S36" s="74"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="74"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="74"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="23"/>
       <c r="X36" s="74"/>
       <c r="Y36" s="74"/>
       <c r="Z36" s="74"/>
@@ -26782,8 +26830,9 @@
       <c r="BF36" s="74"/>
       <c r="BG36" s="74"/>
       <c r="BH36" s="74"/>
-    </row>
-    <row r="37" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI36" s="74"/>
+    </row>
+    <row r="37" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="74"/>
       <c r="B37" s="74"/>
       <c r="C37" s="22"/>
@@ -26803,10 +26852,10 @@
       <c r="Q37" s="74"/>
       <c r="R37" s="74"/>
       <c r="S37" s="74"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="74"/>
+      <c r="T37" s="74"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="23"/>
       <c r="X37" s="74"/>
       <c r="Y37" s="74"/>
       <c r="Z37" s="74"/>
@@ -26844,8 +26893,9 @@
       <c r="BF37" s="74"/>
       <c r="BG37" s="74"/>
       <c r="BH37" s="74"/>
-    </row>
-    <row r="38" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI37" s="74"/>
+    </row>
+    <row r="38" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="74"/>
       <c r="B38" s="74"/>
       <c r="C38" s="22"/>
@@ -26865,10 +26915,10 @@
       <c r="Q38" s="74"/>
       <c r="R38" s="74"/>
       <c r="S38" s="74"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="74"/>
+      <c r="T38" s="74"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="23"/>
       <c r="X38" s="74"/>
       <c r="Y38" s="74"/>
       <c r="Z38" s="74"/>
@@ -26906,8 +26956,9 @@
       <c r="BF38" s="74"/>
       <c r="BG38" s="74"/>
       <c r="BH38" s="74"/>
-    </row>
-    <row r="39" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI38" s="74"/>
+    </row>
+    <row r="39" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="74"/>
       <c r="B39" s="74"/>
       <c r="C39" s="22"/>
@@ -26927,10 +26978,10 @@
       <c r="Q39" s="74"/>
       <c r="R39" s="74"/>
       <c r="S39" s="74"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="74"/>
+      <c r="T39" s="74"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="23"/>
       <c r="X39" s="74"/>
       <c r="Y39" s="74"/>
       <c r="Z39" s="74"/>
@@ -26968,8 +27019,9 @@
       <c r="BF39" s="74"/>
       <c r="BG39" s="74"/>
       <c r="BH39" s="74"/>
-    </row>
-    <row r="40" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI39" s="74"/>
+    </row>
+    <row r="40" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="74"/>
       <c r="B40" s="74"/>
       <c r="C40" s="22"/>
@@ -26989,10 +27041,10 @@
       <c r="Q40" s="74"/>
       <c r="R40" s="74"/>
       <c r="S40" s="74"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="74"/>
+      <c r="T40" s="74"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="23"/>
       <c r="X40" s="74"/>
       <c r="Y40" s="74"/>
       <c r="Z40" s="74"/>
@@ -27030,8 +27082,9 @@
       <c r="BF40" s="74"/>
       <c r="BG40" s="74"/>
       <c r="BH40" s="74"/>
-    </row>
-    <row r="41" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI40" s="74"/>
+    </row>
+    <row r="41" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="74"/>
       <c r="B41" s="74"/>
       <c r="C41" s="22"/>
@@ -27051,10 +27104,10 @@
       <c r="Q41" s="74"/>
       <c r="R41" s="74"/>
       <c r="S41" s="74"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="74"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="23"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="23"/>
       <c r="X41" s="74"/>
       <c r="Y41" s="74"/>
       <c r="Z41" s="74"/>
@@ -27092,8 +27145,9 @@
       <c r="BF41" s="74"/>
       <c r="BG41" s="74"/>
       <c r="BH41" s="74"/>
-    </row>
-    <row r="42" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI41" s="74"/>
+    </row>
+    <row r="42" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="74"/>
       <c r="B42" s="74"/>
       <c r="C42" s="22"/>
@@ -27113,10 +27167,10 @@
       <c r="Q42" s="74"/>
       <c r="R42" s="74"/>
       <c r="S42" s="74"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="23"/>
       <c r="X42" s="74"/>
       <c r="Y42" s="74"/>
       <c r="Z42" s="74"/>
@@ -27154,8 +27208,9 @@
       <c r="BF42" s="74"/>
       <c r="BG42" s="74"/>
       <c r="BH42" s="74"/>
-    </row>
-    <row r="43" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI42" s="74"/>
+    </row>
+    <row r="43" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74"/>
       <c r="B43" s="74"/>
       <c r="C43" s="22"/>
@@ -27175,10 +27230,10 @@
       <c r="Q43" s="74"/>
       <c r="R43" s="74"/>
       <c r="S43" s="74"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="74"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="23"/>
       <c r="X43" s="74"/>
       <c r="Y43" s="74"/>
       <c r="Z43" s="74"/>
@@ -27216,8 +27271,9 @@
       <c r="BF43" s="74"/>
       <c r="BG43" s="74"/>
       <c r="BH43" s="74"/>
-    </row>
-    <row r="44" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI43" s="74"/>
+    </row>
+    <row r="44" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="74"/>
       <c r="B44" s="74"/>
       <c r="C44" s="22"/>
@@ -27237,10 +27293,10 @@
       <c r="Q44" s="74"/>
       <c r="R44" s="74"/>
       <c r="S44" s="74"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="74"/>
+      <c r="T44" s="74"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="74"/>
+      <c r="W44" s="23"/>
       <c r="X44" s="74"/>
       <c r="Y44" s="74"/>
       <c r="Z44" s="74"/>
@@ -27278,8 +27334,9 @@
       <c r="BF44" s="74"/>
       <c r="BG44" s="74"/>
       <c r="BH44" s="74"/>
-    </row>
-    <row r="45" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI44" s="74"/>
+    </row>
+    <row r="45" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74"/>
       <c r="B45" s="74"/>
       <c r="C45" s="22"/>
@@ -27299,10 +27356,10 @@
       <c r="Q45" s="74"/>
       <c r="R45" s="74"/>
       <c r="S45" s="74"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="74"/>
+      <c r="T45" s="74"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="23"/>
       <c r="X45" s="74"/>
       <c r="Y45" s="74"/>
       <c r="Z45" s="74"/>
@@ -27340,8 +27397,9 @@
       <c r="BF45" s="74"/>
       <c r="BG45" s="74"/>
       <c r="BH45" s="74"/>
-    </row>
-    <row r="46" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI45" s="74"/>
+    </row>
+    <row r="46" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74"/>
       <c r="B46" s="74"/>
       <c r="C46" s="22"/>
@@ -27361,10 +27419,10 @@
       <c r="Q46" s="74"/>
       <c r="R46" s="74"/>
       <c r="S46" s="74"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="74"/>
+      <c r="T46" s="74"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="74"/>
+      <c r="W46" s="23"/>
       <c r="X46" s="74"/>
       <c r="Y46" s="74"/>
       <c r="Z46" s="74"/>
@@ -27402,8 +27460,9 @@
       <c r="BF46" s="74"/>
       <c r="BG46" s="74"/>
       <c r="BH46" s="74"/>
-    </row>
-    <row r="47" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI46" s="74"/>
+    </row>
+    <row r="47" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="74"/>
       <c r="B47" s="74"/>
       <c r="C47" s="22"/>
@@ -27423,10 +27482,10 @@
       <c r="Q47" s="74"/>
       <c r="R47" s="74"/>
       <c r="S47" s="74"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="74"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="74"/>
+      <c r="T47" s="74"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="74"/>
+      <c r="W47" s="23"/>
       <c r="X47" s="74"/>
       <c r="Y47" s="74"/>
       <c r="Z47" s="74"/>
@@ -27464,8 +27523,9 @@
       <c r="BF47" s="74"/>
       <c r="BG47" s="74"/>
       <c r="BH47" s="74"/>
-    </row>
-    <row r="48" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI47" s="74"/>
+    </row>
+    <row r="48" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="74"/>
       <c r="B48" s="74"/>
       <c r="C48" s="22"/>
@@ -27485,10 +27545,10 @@
       <c r="Q48" s="74"/>
       <c r="R48" s="74"/>
       <c r="S48" s="74"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="74"/>
-      <c r="V48" s="23"/>
-      <c r="W48" s="74"/>
+      <c r="T48" s="74"/>
+      <c r="U48" s="23"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="23"/>
       <c r="X48" s="74"/>
       <c r="Y48" s="74"/>
       <c r="Z48" s="74"/>
@@ -27526,8 +27586,9 @@
       <c r="BF48" s="74"/>
       <c r="BG48" s="74"/>
       <c r="BH48" s="74"/>
-    </row>
-    <row r="49" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI48" s="74"/>
+    </row>
+    <row r="49" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="74"/>
       <c r="B49" s="74"/>
       <c r="C49" s="22"/>
@@ -27547,10 +27608,10 @@
       <c r="Q49" s="74"/>
       <c r="R49" s="74"/>
       <c r="S49" s="74"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="74"/>
-      <c r="V49" s="23"/>
-      <c r="W49" s="74"/>
+      <c r="T49" s="74"/>
+      <c r="U49" s="23"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="23"/>
       <c r="X49" s="74"/>
       <c r="Y49" s="74"/>
       <c r="Z49" s="74"/>
@@ -27588,8 +27649,9 @@
       <c r="BF49" s="74"/>
       <c r="BG49" s="74"/>
       <c r="BH49" s="74"/>
-    </row>
-    <row r="50" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI49" s="74"/>
+    </row>
+    <row r="50" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="74"/>
       <c r="B50" s="74"/>
       <c r="C50" s="22"/>
@@ -27609,10 +27671,10 @@
       <c r="Q50" s="74"/>
       <c r="R50" s="74"/>
       <c r="S50" s="74"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="74"/>
-      <c r="V50" s="23"/>
-      <c r="W50" s="74"/>
+      <c r="T50" s="74"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="23"/>
       <c r="X50" s="74"/>
       <c r="Y50" s="74"/>
       <c r="Z50" s="74"/>
@@ -27650,8 +27712,9 @@
       <c r="BF50" s="74"/>
       <c r="BG50" s="74"/>
       <c r="BH50" s="74"/>
-    </row>
-    <row r="51" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI50" s="74"/>
+    </row>
+    <row r="51" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="74"/>
       <c r="B51" s="74"/>
       <c r="C51" s="22"/>
@@ -27671,10 +27734,10 @@
       <c r="Q51" s="74"/>
       <c r="R51" s="74"/>
       <c r="S51" s="74"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="23"/>
-      <c r="W51" s="74"/>
+      <c r="T51" s="74"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="74"/>
+      <c r="W51" s="23"/>
       <c r="X51" s="74"/>
       <c r="Y51" s="74"/>
       <c r="Z51" s="74"/>
@@ -27712,8 +27775,9 @@
       <c r="BF51" s="74"/>
       <c r="BG51" s="74"/>
       <c r="BH51" s="74"/>
-    </row>
-    <row r="52" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI51" s="74"/>
+    </row>
+    <row r="52" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="74"/>
       <c r="B52" s="74"/>
       <c r="C52" s="22"/>
@@ -27733,10 +27797,10 @@
       <c r="Q52" s="74"/>
       <c r="R52" s="74"/>
       <c r="S52" s="74"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="74"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="74"/>
+      <c r="T52" s="74"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="74"/>
+      <c r="W52" s="23"/>
       <c r="X52" s="74"/>
       <c r="Y52" s="74"/>
       <c r="Z52" s="74"/>
@@ -27774,8 +27838,9 @@
       <c r="BF52" s="74"/>
       <c r="BG52" s="74"/>
       <c r="BH52" s="74"/>
-    </row>
-    <row r="53" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI52" s="74"/>
+    </row>
+    <row r="53" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="74"/>
       <c r="B53" s="74"/>
       <c r="C53" s="22"/>
@@ -27795,10 +27860,10 @@
       <c r="Q53" s="74"/>
       <c r="R53" s="74"/>
       <c r="S53" s="74"/>
-      <c r="T53" s="23"/>
-      <c r="U53" s="74"/>
-      <c r="V53" s="23"/>
-      <c r="W53" s="74"/>
+      <c r="T53" s="74"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="74"/>
+      <c r="W53" s="23"/>
       <c r="X53" s="74"/>
       <c r="Y53" s="74"/>
       <c r="Z53" s="74"/>
@@ -27836,8 +27901,9 @@
       <c r="BF53" s="74"/>
       <c r="BG53" s="74"/>
       <c r="BH53" s="74"/>
-    </row>
-    <row r="54" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI53" s="74"/>
+    </row>
+    <row r="54" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="74"/>
       <c r="B54" s="74"/>
       <c r="C54" s="22"/>
@@ -27857,10 +27923,10 @@
       <c r="Q54" s="74"/>
       <c r="R54" s="74"/>
       <c r="S54" s="74"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="74"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="74"/>
+      <c r="T54" s="74"/>
+      <c r="U54" s="23"/>
+      <c r="V54" s="74"/>
+      <c r="W54" s="23"/>
       <c r="X54" s="74"/>
       <c r="Y54" s="74"/>
       <c r="Z54" s="74"/>
@@ -27898,8 +27964,9 @@
       <c r="BF54" s="74"/>
       <c r="BG54" s="74"/>
       <c r="BH54" s="74"/>
-    </row>
-    <row r="55" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI54" s="74"/>
+    </row>
+    <row r="55" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="74"/>
       <c r="B55" s="74"/>
       <c r="C55" s="22"/>
@@ -27919,10 +27986,10 @@
       <c r="Q55" s="74"/>
       <c r="R55" s="74"/>
       <c r="S55" s="74"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="74"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="74"/>
+      <c r="T55" s="74"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="74"/>
+      <c r="W55" s="23"/>
       <c r="X55" s="74"/>
       <c r="Y55" s="74"/>
       <c r="Z55" s="74"/>
@@ -27960,8 +28027,9 @@
       <c r="BF55" s="74"/>
       <c r="BG55" s="74"/>
       <c r="BH55" s="74"/>
-    </row>
-    <row r="56" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI55" s="74"/>
+    </row>
+    <row r="56" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="74"/>
       <c r="B56" s="74"/>
       <c r="C56" s="22"/>
@@ -27981,10 +28049,10 @@
       <c r="Q56" s="74"/>
       <c r="R56" s="74"/>
       <c r="S56" s="74"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="74"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="74"/>
+      <c r="T56" s="74"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="74"/>
+      <c r="W56" s="23"/>
       <c r="X56" s="74"/>
       <c r="Y56" s="74"/>
       <c r="Z56" s="74"/>
@@ -28022,8 +28090,9 @@
       <c r="BF56" s="74"/>
       <c r="BG56" s="74"/>
       <c r="BH56" s="74"/>
-    </row>
-    <row r="57" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI56" s="74"/>
+    </row>
+    <row r="57" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="74"/>
       <c r="B57" s="74"/>
       <c r="C57" s="22"/>
@@ -28043,10 +28112,10 @@
       <c r="Q57" s="74"/>
       <c r="R57" s="74"/>
       <c r="S57" s="74"/>
-      <c r="T57" s="23"/>
-      <c r="U57" s="74"/>
-      <c r="V57" s="23"/>
-      <c r="W57" s="74"/>
+      <c r="T57" s="74"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="74"/>
+      <c r="W57" s="23"/>
       <c r="X57" s="74"/>
       <c r="Y57" s="74"/>
       <c r="Z57" s="74"/>
@@ -28084,8 +28153,9 @@
       <c r="BF57" s="74"/>
       <c r="BG57" s="74"/>
       <c r="BH57" s="74"/>
-    </row>
-    <row r="58" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI57" s="74"/>
+    </row>
+    <row r="58" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="74"/>
       <c r="B58" s="74"/>
       <c r="C58" s="22"/>
@@ -28105,10 +28175,10 @@
       <c r="Q58" s="74"/>
       <c r="R58" s="74"/>
       <c r="S58" s="74"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="74"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="74"/>
+      <c r="T58" s="74"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="74"/>
+      <c r="W58" s="23"/>
       <c r="X58" s="74"/>
       <c r="Y58" s="74"/>
       <c r="Z58" s="74"/>
@@ -28146,8 +28216,9 @@
       <c r="BF58" s="74"/>
       <c r="BG58" s="74"/>
       <c r="BH58" s="74"/>
-    </row>
-    <row r="59" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI58" s="74"/>
+    </row>
+    <row r="59" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="74"/>
       <c r="B59" s="74"/>
       <c r="C59" s="22"/>
@@ -28167,10 +28238,10 @@
       <c r="Q59" s="74"/>
       <c r="R59" s="74"/>
       <c r="S59" s="74"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="74"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="74"/>
+      <c r="T59" s="74"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="74"/>
+      <c r="W59" s="23"/>
       <c r="X59" s="74"/>
       <c r="Y59" s="74"/>
       <c r="Z59" s="74"/>
@@ -28208,8 +28279,9 @@
       <c r="BF59" s="74"/>
       <c r="BG59" s="74"/>
       <c r="BH59" s="74"/>
-    </row>
-    <row r="60" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI59" s="74"/>
+    </row>
+    <row r="60" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="74"/>
       <c r="B60" s="74"/>
       <c r="C60" s="22"/>
@@ -28229,10 +28301,10 @@
       <c r="Q60" s="74"/>
       <c r="R60" s="74"/>
       <c r="S60" s="74"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="74"/>
-      <c r="V60" s="23"/>
-      <c r="W60" s="74"/>
+      <c r="T60" s="74"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="74"/>
+      <c r="W60" s="23"/>
       <c r="X60" s="74"/>
       <c r="Y60" s="74"/>
       <c r="Z60" s="74"/>
@@ -28270,8 +28342,9 @@
       <c r="BF60" s="74"/>
       <c r="BG60" s="74"/>
       <c r="BH60" s="74"/>
-    </row>
-    <row r="61" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI60" s="74"/>
+    </row>
+    <row r="61" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="74"/>
       <c r="B61" s="74"/>
       <c r="C61" s="22"/>
@@ -28291,10 +28364,10 @@
       <c r="Q61" s="74"/>
       <c r="R61" s="74"/>
       <c r="S61" s="74"/>
-      <c r="T61" s="23"/>
-      <c r="U61" s="74"/>
-      <c r="V61" s="23"/>
-      <c r="W61" s="74"/>
+      <c r="T61" s="74"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="74"/>
+      <c r="W61" s="23"/>
       <c r="X61" s="74"/>
       <c r="Y61" s="74"/>
       <c r="Z61" s="74"/>
@@ -28332,8 +28405,9 @@
       <c r="BF61" s="74"/>
       <c r="BG61" s="74"/>
       <c r="BH61" s="74"/>
-    </row>
-    <row r="62" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI61" s="74"/>
+    </row>
+    <row r="62" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="74"/>
       <c r="B62" s="74"/>
       <c r="C62" s="22"/>
@@ -28353,10 +28427,10 @@
       <c r="Q62" s="74"/>
       <c r="R62" s="74"/>
       <c r="S62" s="74"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="74"/>
-      <c r="V62" s="23"/>
-      <c r="W62" s="74"/>
+      <c r="T62" s="74"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="74"/>
+      <c r="W62" s="23"/>
       <c r="X62" s="74"/>
       <c r="Y62" s="74"/>
       <c r="Z62" s="74"/>
@@ -28394,8 +28468,9 @@
       <c r="BF62" s="74"/>
       <c r="BG62" s="74"/>
       <c r="BH62" s="74"/>
-    </row>
-    <row r="63" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI62" s="74"/>
+    </row>
+    <row r="63" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="74"/>
       <c r="B63" s="74"/>
       <c r="C63" s="22"/>
@@ -28415,10 +28490,10 @@
       <c r="Q63" s="74"/>
       <c r="R63" s="74"/>
       <c r="S63" s="74"/>
-      <c r="T63" s="23"/>
-      <c r="U63" s="74"/>
-      <c r="V63" s="23"/>
-      <c r="W63" s="74"/>
+      <c r="T63" s="74"/>
+      <c r="U63" s="23"/>
+      <c r="V63" s="74"/>
+      <c r="W63" s="23"/>
       <c r="X63" s="74"/>
       <c r="Y63" s="74"/>
       <c r="Z63" s="74"/>
@@ -28456,8 +28531,9 @@
       <c r="BF63" s="74"/>
       <c r="BG63" s="74"/>
       <c r="BH63" s="74"/>
-    </row>
-    <row r="64" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI63" s="74"/>
+    </row>
+    <row r="64" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="74"/>
       <c r="B64" s="74"/>
       <c r="C64" s="22"/>
@@ -28477,10 +28553,10 @@
       <c r="Q64" s="74"/>
       <c r="R64" s="74"/>
       <c r="S64" s="74"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="74"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="74"/>
+      <c r="T64" s="74"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="74"/>
+      <c r="W64" s="23"/>
       <c r="X64" s="74"/>
       <c r="Y64" s="74"/>
       <c r="Z64" s="74"/>
@@ -28518,8 +28594,9 @@
       <c r="BF64" s="74"/>
       <c r="BG64" s="74"/>
       <c r="BH64" s="74"/>
-    </row>
-    <row r="65" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI64" s="74"/>
+    </row>
+    <row r="65" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="74"/>
       <c r="B65" s="74"/>
       <c r="C65" s="22"/>
@@ -28539,10 +28616,10 @@
       <c r="Q65" s="74"/>
       <c r="R65" s="74"/>
       <c r="S65" s="74"/>
-      <c r="T65" s="23"/>
-      <c r="U65" s="74"/>
-      <c r="V65" s="23"/>
-      <c r="W65" s="74"/>
+      <c r="T65" s="74"/>
+      <c r="U65" s="23"/>
+      <c r="V65" s="74"/>
+      <c r="W65" s="23"/>
       <c r="X65" s="74"/>
       <c r="Y65" s="74"/>
       <c r="Z65" s="74"/>
@@ -28580,8 +28657,9 @@
       <c r="BF65" s="74"/>
       <c r="BG65" s="74"/>
       <c r="BH65" s="74"/>
-    </row>
-    <row r="66" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI65" s="74"/>
+    </row>
+    <row r="66" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="74"/>
       <c r="B66" s="74"/>
       <c r="C66" s="22"/>
@@ -28601,10 +28679,10 @@
       <c r="Q66" s="74"/>
       <c r="R66" s="74"/>
       <c r="S66" s="74"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="74"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="74"/>
+      <c r="T66" s="74"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="74"/>
+      <c r="W66" s="23"/>
       <c r="X66" s="74"/>
       <c r="Y66" s="74"/>
       <c r="Z66" s="74"/>
@@ -28642,8 +28720,9 @@
       <c r="BF66" s="74"/>
       <c r="BG66" s="74"/>
       <c r="BH66" s="74"/>
-    </row>
-    <row r="67" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI66" s="74"/>
+    </row>
+    <row r="67" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="74"/>
       <c r="B67" s="74"/>
       <c r="C67" s="22"/>
@@ -28663,10 +28742,10 @@
       <c r="Q67" s="74"/>
       <c r="R67" s="74"/>
       <c r="S67" s="74"/>
-      <c r="T67" s="23"/>
-      <c r="U67" s="74"/>
-      <c r="V67" s="23"/>
-      <c r="W67" s="74"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="74"/>
+      <c r="W67" s="23"/>
       <c r="X67" s="74"/>
       <c r="Y67" s="74"/>
       <c r="Z67" s="74"/>
@@ -28704,8 +28783,9 @@
       <c r="BF67" s="74"/>
       <c r="BG67" s="74"/>
       <c r="BH67" s="74"/>
-    </row>
-    <row r="68" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI67" s="74"/>
+    </row>
+    <row r="68" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="74"/>
       <c r="B68" s="74"/>
       <c r="C68" s="22"/>
@@ -28725,10 +28805,10 @@
       <c r="Q68" s="74"/>
       <c r="R68" s="74"/>
       <c r="S68" s="74"/>
-      <c r="T68" s="23"/>
-      <c r="U68" s="74"/>
-      <c r="V68" s="23"/>
-      <c r="W68" s="74"/>
+      <c r="T68" s="74"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="74"/>
+      <c r="W68" s="23"/>
       <c r="X68" s="74"/>
       <c r="Y68" s="74"/>
       <c r="Z68" s="74"/>
@@ -28766,8 +28846,9 @@
       <c r="BF68" s="74"/>
       <c r="BG68" s="74"/>
       <c r="BH68" s="74"/>
-    </row>
-    <row r="69" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI68" s="74"/>
+    </row>
+    <row r="69" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="74"/>
       <c r="B69" s="74"/>
       <c r="C69" s="22"/>
@@ -28787,10 +28868,10 @@
       <c r="Q69" s="74"/>
       <c r="R69" s="74"/>
       <c r="S69" s="74"/>
-      <c r="T69" s="23"/>
-      <c r="U69" s="74"/>
-      <c r="V69" s="23"/>
-      <c r="W69" s="74"/>
+      <c r="T69" s="74"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="74"/>
+      <c r="W69" s="23"/>
       <c r="X69" s="74"/>
       <c r="Y69" s="74"/>
       <c r="Z69" s="74"/>
@@ -28828,8 +28909,9 @@
       <c r="BF69" s="74"/>
       <c r="BG69" s="74"/>
       <c r="BH69" s="74"/>
-    </row>
-    <row r="70" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI69" s="74"/>
+    </row>
+    <row r="70" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="74"/>
       <c r="B70" s="74"/>
       <c r="C70" s="22"/>
@@ -28849,10 +28931,10 @@
       <c r="Q70" s="74"/>
       <c r="R70" s="74"/>
       <c r="S70" s="74"/>
-      <c r="T70" s="23"/>
-      <c r="U70" s="74"/>
-      <c r="V70" s="23"/>
-      <c r="W70" s="74"/>
+      <c r="T70" s="74"/>
+      <c r="U70" s="23"/>
+      <c r="V70" s="74"/>
+      <c r="W70" s="23"/>
       <c r="X70" s="74"/>
       <c r="Y70" s="74"/>
       <c r="Z70" s="74"/>
@@ -28890,8 +28972,9 @@
       <c r="BF70" s="74"/>
       <c r="BG70" s="74"/>
       <c r="BH70" s="74"/>
-    </row>
-    <row r="71" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI70" s="74"/>
+    </row>
+    <row r="71" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="74"/>
       <c r="B71" s="74"/>
       <c r="C71" s="22"/>
@@ -28911,10 +28994,10 @@
       <c r="Q71" s="74"/>
       <c r="R71" s="74"/>
       <c r="S71" s="74"/>
-      <c r="T71" s="23"/>
-      <c r="U71" s="74"/>
-      <c r="V71" s="23"/>
-      <c r="W71" s="74"/>
+      <c r="T71" s="74"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="74"/>
+      <c r="W71" s="23"/>
       <c r="X71" s="74"/>
       <c r="Y71" s="74"/>
       <c r="Z71" s="74"/>
@@ -28952,8 +29035,9 @@
       <c r="BF71" s="74"/>
       <c r="BG71" s="74"/>
       <c r="BH71" s="74"/>
-    </row>
-    <row r="72" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI71" s="74"/>
+    </row>
+    <row r="72" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="74"/>
       <c r="B72" s="74"/>
       <c r="C72" s="22"/>
@@ -28973,10 +29057,10 @@
       <c r="Q72" s="74"/>
       <c r="R72" s="74"/>
       <c r="S72" s="74"/>
-      <c r="T72" s="23"/>
-      <c r="U72" s="74"/>
-      <c r="V72" s="23"/>
-      <c r="W72" s="74"/>
+      <c r="T72" s="74"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="74"/>
+      <c r="W72" s="23"/>
       <c r="X72" s="74"/>
       <c r="Y72" s="74"/>
       <c r="Z72" s="74"/>
@@ -29014,8 +29098,9 @@
       <c r="BF72" s="74"/>
       <c r="BG72" s="74"/>
       <c r="BH72" s="74"/>
-    </row>
-    <row r="73" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI72" s="74"/>
+    </row>
+    <row r="73" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="74"/>
       <c r="B73" s="74"/>
       <c r="C73" s="22"/>
@@ -29035,10 +29120,10 @@
       <c r="Q73" s="74"/>
       <c r="R73" s="74"/>
       <c r="S73" s="74"/>
-      <c r="T73" s="23"/>
-      <c r="U73" s="74"/>
-      <c r="V73" s="23"/>
-      <c r="W73" s="74"/>
+      <c r="T73" s="74"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="74"/>
+      <c r="W73" s="23"/>
       <c r="X73" s="74"/>
       <c r="Y73" s="74"/>
       <c r="Z73" s="74"/>
@@ -29076,8 +29161,9 @@
       <c r="BF73" s="74"/>
       <c r="BG73" s="74"/>
       <c r="BH73" s="74"/>
-    </row>
-    <row r="74" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI73" s="74"/>
+    </row>
+    <row r="74" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="74"/>
       <c r="B74" s="74"/>
       <c r="C74" s="22"/>
@@ -29097,10 +29183,10 @@
       <c r="Q74" s="74"/>
       <c r="R74" s="74"/>
       <c r="S74" s="74"/>
-      <c r="T74" s="23"/>
-      <c r="U74" s="74"/>
-      <c r="V74" s="23"/>
-      <c r="W74" s="74"/>
+      <c r="T74" s="74"/>
+      <c r="U74" s="23"/>
+      <c r="V74" s="74"/>
+      <c r="W74" s="23"/>
       <c r="X74" s="74"/>
       <c r="Y74" s="74"/>
       <c r="Z74" s="74"/>
@@ -29138,8 +29224,9 @@
       <c r="BF74" s="74"/>
       <c r="BG74" s="74"/>
       <c r="BH74" s="74"/>
-    </row>
-    <row r="75" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI74" s="74"/>
+    </row>
+    <row r="75" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="74"/>
       <c r="B75" s="74"/>
       <c r="C75" s="22"/>
@@ -29159,10 +29246,10 @@
       <c r="Q75" s="74"/>
       <c r="R75" s="74"/>
       <c r="S75" s="74"/>
-      <c r="T75" s="23"/>
-      <c r="U75" s="74"/>
-      <c r="V75" s="23"/>
-      <c r="W75" s="74"/>
+      <c r="T75" s="74"/>
+      <c r="U75" s="23"/>
+      <c r="V75" s="74"/>
+      <c r="W75" s="23"/>
       <c r="X75" s="74"/>
       <c r="Y75" s="74"/>
       <c r="Z75" s="74"/>
@@ -29200,8 +29287,9 @@
       <c r="BF75" s="74"/>
       <c r="BG75" s="74"/>
       <c r="BH75" s="74"/>
-    </row>
-    <row r="76" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI75" s="74"/>
+    </row>
+    <row r="76" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="74"/>
       <c r="B76" s="74"/>
       <c r="C76" s="22"/>
@@ -29221,10 +29309,10 @@
       <c r="Q76" s="74"/>
       <c r="R76" s="74"/>
       <c r="S76" s="74"/>
-      <c r="T76" s="23"/>
-      <c r="U76" s="74"/>
-      <c r="V76" s="23"/>
-      <c r="W76" s="74"/>
+      <c r="T76" s="74"/>
+      <c r="U76" s="23"/>
+      <c r="V76" s="74"/>
+      <c r="W76" s="23"/>
       <c r="X76" s="74"/>
       <c r="Y76" s="74"/>
       <c r="Z76" s="74"/>
@@ -29262,8 +29350,9 @@
       <c r="BF76" s="74"/>
       <c r="BG76" s="74"/>
       <c r="BH76" s="74"/>
-    </row>
-    <row r="77" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI76" s="74"/>
+    </row>
+    <row r="77" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="74"/>
       <c r="B77" s="74"/>
       <c r="C77" s="22"/>
@@ -29283,10 +29372,10 @@
       <c r="Q77" s="74"/>
       <c r="R77" s="74"/>
       <c r="S77" s="74"/>
-      <c r="T77" s="23"/>
-      <c r="U77" s="74"/>
-      <c r="V77" s="23"/>
-      <c r="W77" s="74"/>
+      <c r="T77" s="74"/>
+      <c r="U77" s="23"/>
+      <c r="V77" s="74"/>
+      <c r="W77" s="23"/>
       <c r="X77" s="74"/>
       <c r="Y77" s="74"/>
       <c r="Z77" s="74"/>
@@ -29324,8 +29413,9 @@
       <c r="BF77" s="74"/>
       <c r="BG77" s="74"/>
       <c r="BH77" s="74"/>
-    </row>
-    <row r="78" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI77" s="74"/>
+    </row>
+    <row r="78" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="74"/>
       <c r="B78" s="74"/>
       <c r="C78" s="22"/>
@@ -29345,10 +29435,10 @@
       <c r="Q78" s="74"/>
       <c r="R78" s="74"/>
       <c r="S78" s="74"/>
-      <c r="T78" s="23"/>
-      <c r="U78" s="74"/>
-      <c r="V78" s="23"/>
-      <c r="W78" s="74"/>
+      <c r="T78" s="74"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="74"/>
+      <c r="W78" s="23"/>
       <c r="X78" s="74"/>
       <c r="Y78" s="74"/>
       <c r="Z78" s="74"/>
@@ -29386,8 +29476,9 @@
       <c r="BF78" s="74"/>
       <c r="BG78" s="74"/>
       <c r="BH78" s="74"/>
-    </row>
-    <row r="79" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI78" s="74"/>
+    </row>
+    <row r="79" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="74"/>
       <c r="B79" s="74"/>
       <c r="C79" s="22"/>
@@ -29407,10 +29498,10 @@
       <c r="Q79" s="74"/>
       <c r="R79" s="74"/>
       <c r="S79" s="74"/>
-      <c r="T79" s="23"/>
-      <c r="U79" s="74"/>
-      <c r="V79" s="23"/>
-      <c r="W79" s="74"/>
+      <c r="T79" s="74"/>
+      <c r="U79" s="23"/>
+      <c r="V79" s="74"/>
+      <c r="W79" s="23"/>
       <c r="X79" s="74"/>
       <c r="Y79" s="74"/>
       <c r="Z79" s="74"/>
@@ -29448,8 +29539,9 @@
       <c r="BF79" s="74"/>
       <c r="BG79" s="74"/>
       <c r="BH79" s="74"/>
-    </row>
-    <row r="80" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI79" s="74"/>
+    </row>
+    <row r="80" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="74"/>
       <c r="B80" s="74"/>
       <c r="C80" s="22"/>
@@ -29469,10 +29561,10 @@
       <c r="Q80" s="74"/>
       <c r="R80" s="74"/>
       <c r="S80" s="74"/>
-      <c r="T80" s="23"/>
-      <c r="U80" s="74"/>
-      <c r="V80" s="23"/>
-      <c r="W80" s="74"/>
+      <c r="T80" s="74"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="74"/>
+      <c r="W80" s="23"/>
       <c r="X80" s="74"/>
       <c r="Y80" s="74"/>
       <c r="Z80" s="74"/>
@@ -29510,8 +29602,9 @@
       <c r="BF80" s="74"/>
       <c r="BG80" s="74"/>
       <c r="BH80" s="74"/>
-    </row>
-    <row r="81" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI80" s="74"/>
+    </row>
+    <row r="81" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="74"/>
       <c r="B81" s="74"/>
       <c r="C81" s="22"/>
@@ -29531,10 +29624,10 @@
       <c r="Q81" s="74"/>
       <c r="R81" s="74"/>
       <c r="S81" s="74"/>
-      <c r="T81" s="23"/>
-      <c r="U81" s="74"/>
-      <c r="V81" s="23"/>
-      <c r="W81" s="74"/>
+      <c r="T81" s="74"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="74"/>
+      <c r="W81" s="23"/>
       <c r="X81" s="74"/>
       <c r="Y81" s="74"/>
       <c r="Z81" s="74"/>
@@ -29572,8 +29665,9 @@
       <c r="BF81" s="74"/>
       <c r="BG81" s="74"/>
       <c r="BH81" s="74"/>
-    </row>
-    <row r="82" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI81" s="74"/>
+    </row>
+    <row r="82" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="74"/>
       <c r="B82" s="74"/>
       <c r="C82" s="22"/>
@@ -29593,10 +29687,10 @@
       <c r="Q82" s="74"/>
       <c r="R82" s="74"/>
       <c r="S82" s="74"/>
-      <c r="T82" s="23"/>
-      <c r="U82" s="74"/>
-      <c r="V82" s="23"/>
-      <c r="W82" s="74"/>
+      <c r="T82" s="74"/>
+      <c r="U82" s="23"/>
+      <c r="V82" s="74"/>
+      <c r="W82" s="23"/>
       <c r="X82" s="74"/>
       <c r="Y82" s="74"/>
       <c r="Z82" s="74"/>
@@ -29634,8 +29728,9 @@
       <c r="BF82" s="74"/>
       <c r="BG82" s="74"/>
       <c r="BH82" s="74"/>
-    </row>
-    <row r="83" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI82" s="74"/>
+    </row>
+    <row r="83" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="74"/>
       <c r="B83" s="74"/>
       <c r="C83" s="22"/>
@@ -29655,10 +29750,10 @@
       <c r="Q83" s="74"/>
       <c r="R83" s="74"/>
       <c r="S83" s="74"/>
-      <c r="T83" s="23"/>
-      <c r="U83" s="74"/>
-      <c r="V83" s="23"/>
-      <c r="W83" s="74"/>
+      <c r="T83" s="74"/>
+      <c r="U83" s="23"/>
+      <c r="V83" s="74"/>
+      <c r="W83" s="23"/>
       <c r="X83" s="74"/>
       <c r="Y83" s="74"/>
       <c r="Z83" s="74"/>
@@ -29696,8 +29791,9 @@
       <c r="BF83" s="74"/>
       <c r="BG83" s="74"/>
       <c r="BH83" s="74"/>
-    </row>
-    <row r="84" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI83" s="74"/>
+    </row>
+    <row r="84" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="74"/>
       <c r="B84" s="74"/>
       <c r="C84" s="22"/>
@@ -29717,10 +29813,10 @@
       <c r="Q84" s="74"/>
       <c r="R84" s="74"/>
       <c r="S84" s="74"/>
-      <c r="T84" s="23"/>
-      <c r="U84" s="74"/>
-      <c r="V84" s="23"/>
-      <c r="W84" s="74"/>
+      <c r="T84" s="74"/>
+      <c r="U84" s="23"/>
+      <c r="V84" s="74"/>
+      <c r="W84" s="23"/>
       <c r="X84" s="74"/>
       <c r="Y84" s="74"/>
       <c r="Z84" s="74"/>
@@ -29758,8 +29854,9 @@
       <c r="BF84" s="74"/>
       <c r="BG84" s="74"/>
       <c r="BH84" s="74"/>
-    </row>
-    <row r="85" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI84" s="74"/>
+    </row>
+    <row r="85" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="74"/>
       <c r="B85" s="74"/>
       <c r="C85" s="22"/>
@@ -29779,10 +29876,10 @@
       <c r="Q85" s="74"/>
       <c r="R85" s="74"/>
       <c r="S85" s="74"/>
-      <c r="T85" s="23"/>
-      <c r="U85" s="74"/>
-      <c r="V85" s="23"/>
-      <c r="W85" s="74"/>
+      <c r="T85" s="74"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="74"/>
+      <c r="W85" s="23"/>
       <c r="X85" s="74"/>
       <c r="Y85" s="74"/>
       <c r="Z85" s="74"/>
@@ -29820,8 +29917,9 @@
       <c r="BF85" s="74"/>
       <c r="BG85" s="74"/>
       <c r="BH85" s="74"/>
-    </row>
-    <row r="86" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI85" s="74"/>
+    </row>
+    <row r="86" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="74"/>
       <c r="B86" s="74"/>
       <c r="C86" s="22"/>
@@ -29841,10 +29939,10 @@
       <c r="Q86" s="74"/>
       <c r="R86" s="74"/>
       <c r="S86" s="74"/>
-      <c r="T86" s="23"/>
-      <c r="U86" s="74"/>
-      <c r="V86" s="23"/>
-      <c r="W86" s="74"/>
+      <c r="T86" s="74"/>
+      <c r="U86" s="23"/>
+      <c r="V86" s="74"/>
+      <c r="W86" s="23"/>
       <c r="X86" s="74"/>
       <c r="Y86" s="74"/>
       <c r="Z86" s="74"/>
@@ -29882,8 +29980,9 @@
       <c r="BF86" s="74"/>
       <c r="BG86" s="74"/>
       <c r="BH86" s="74"/>
-    </row>
-    <row r="87" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI86" s="74"/>
+    </row>
+    <row r="87" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="74"/>
       <c r="B87" s="74"/>
       <c r="C87" s="22"/>
@@ -29903,10 +30002,10 @@
       <c r="Q87" s="74"/>
       <c r="R87" s="74"/>
       <c r="S87" s="74"/>
-      <c r="T87" s="23"/>
-      <c r="U87" s="74"/>
-      <c r="V87" s="23"/>
-      <c r="W87" s="74"/>
+      <c r="T87" s="74"/>
+      <c r="U87" s="23"/>
+      <c r="V87" s="74"/>
+      <c r="W87" s="23"/>
       <c r="X87" s="74"/>
       <c r="Y87" s="74"/>
       <c r="Z87" s="74"/>
@@ -29944,8 +30043,9 @@
       <c r="BF87" s="74"/>
       <c r="BG87" s="74"/>
       <c r="BH87" s="74"/>
-    </row>
-    <row r="88" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI87" s="74"/>
+    </row>
+    <row r="88" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="74"/>
       <c r="B88" s="74"/>
       <c r="C88" s="22"/>
@@ -30006,8 +30106,9 @@
       <c r="BF88" s="74"/>
       <c r="BG88" s="74"/>
       <c r="BH88" s="74"/>
-    </row>
-    <row r="89" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI88" s="74"/>
+    </row>
+    <row r="89" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="74"/>
       <c r="B89" s="74"/>
       <c r="C89" s="22"/>
@@ -30068,8 +30169,9 @@
       <c r="BF89" s="74"/>
       <c r="BG89" s="74"/>
       <c r="BH89" s="74"/>
-    </row>
-    <row r="90" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI89" s="74"/>
+    </row>
+    <row r="90" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="74"/>
       <c r="B90" s="74"/>
       <c r="C90" s="22"/>
@@ -30130,8 +30232,9 @@
       <c r="BF90" s="74"/>
       <c r="BG90" s="74"/>
       <c r="BH90" s="74"/>
-    </row>
-    <row r="91" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI90" s="74"/>
+    </row>
+    <row r="91" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="74"/>
       <c r="B91" s="74"/>
       <c r="C91" s="22"/>
@@ -30192,8 +30295,9 @@
       <c r="BF91" s="74"/>
       <c r="BG91" s="74"/>
       <c r="BH91" s="74"/>
-    </row>
-    <row r="92" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI91" s="74"/>
+    </row>
+    <row r="92" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="74"/>
       <c r="B92" s="74"/>
       <c r="C92" s="22"/>
@@ -30254,8 +30358,9 @@
       <c r="BF92" s="74"/>
       <c r="BG92" s="74"/>
       <c r="BH92" s="74"/>
-    </row>
-    <row r="93" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI92" s="74"/>
+    </row>
+    <row r="93" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="74"/>
       <c r="B93" s="74"/>
       <c r="C93" s="22"/>
@@ -30316,8 +30421,9 @@
       <c r="BF93" s="74"/>
       <c r="BG93" s="74"/>
       <c r="BH93" s="74"/>
-    </row>
-    <row r="94" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI93" s="74"/>
+    </row>
+    <row r="94" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="74"/>
       <c r="B94" s="74"/>
       <c r="C94" s="22"/>
@@ -30378,8 +30484,9 @@
       <c r="BF94" s="74"/>
       <c r="BG94" s="74"/>
       <c r="BH94" s="74"/>
-    </row>
-    <row r="95" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI94" s="74"/>
+    </row>
+    <row r="95" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="74"/>
       <c r="B95" s="74"/>
       <c r="C95" s="22"/>
@@ -30440,6 +30547,7 @@
       <c r="BF95" s="74"/>
       <c r="BG95" s="74"/>
       <c r="BH95" s="74"/>
+      <c r="BI95" s="74"/>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -30452,22 +30560,22 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E95" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R87" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S87" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Resident,Migratory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S87" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T87" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Rough guess (guesstimate),Ad hoc or opportunistic monitoring,Formal survey/census: total count (the total reserve sampled in an attempt to count all individuals present,e.g.,helicopter total count),Formal survey/census: total population estimated from s"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U87" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V87" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Aerial census - sample count (transects or blocks),Aerial census - total count – fixed wing,Aerial census – total count – helicopter,Call-up survey,Camera trap survey – with density estimation (e.g.,capture/recapture),Camera trap survey – without density"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W87" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X87" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Low/poor: only a small number of sample units (transects,camera traps,etc) that cover a small part of the reserve or are biased to certain areas,Medium/fair: sample units (transects,camera traps,etc) cover a fair proportion of the reserve and are fair"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{00000000-0002-0000-0200-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,2,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X95" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y95" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix subpopulation fields (#1593)
* add adult_total field

* add adult_total to excel upload logic

* update subpopulation fields online form

* remove data template zone identifier file
</commit_message>
<xml_diff>
--- a/django_project/frontend/tests/csv/excel_error_property.xlsx
+++ b/django_project/frontend/tests/csv/excel_error_property.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Impt Backup\sanbi\test_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3599134-8E3F-4EEE-AC20-08F29AF1AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2CAC7A-93CC-4E88-916F-C31C82D412C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="4155" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,11 @@
     <sheet name="Scientific name dropdown" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7142" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7143" uniqueCount="622">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -1918,6 +1917,9 @@
   </si>
   <si>
     <t>Property_code</t>
+  </si>
+  <si>
+    <t>COUNT_adult_TOTAL</t>
   </si>
 </sst>
 </file>
@@ -24334,10 +24336,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BH95"/>
+  <dimension ref="A1:BI95"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24346,15 +24348,22 @@
     <col min="2" max="2" width="15.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="4" customWidth="1"/>
     <col min="4" max="6" width="21.7109375" style="4" customWidth="1"/>
-    <col min="7" max="18" width="8.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="40.85546875" style="4" customWidth="1"/>
-    <col min="20" max="21" width="8.42578125" style="4" customWidth="1"/>
-    <col min="22" max="23" width="30.28515625" style="4" customWidth="1"/>
-    <col min="24" max="61" width="8.42578125" style="4" customWidth="1"/>
-    <col min="62" max="16384" width="8.42578125" style="4"/>
+    <col min="7" max="7" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="8.42578125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="40.85546875" style="4" customWidth="1"/>
+    <col min="21" max="22" width="8.42578125" style="4" customWidth="1"/>
+    <col min="23" max="24" width="30.28515625" style="4" customWidth="1"/>
+    <col min="25" max="62" width="8.42578125" style="4" customWidth="1"/>
+    <col min="63" max="16384" width="8.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="87" t="s">
         <v>620</v>
       </c>
@@ -24377,166 +24386,169 @@
         <v>32</v>
       </c>
       <c r="H1" s="94" t="s">
+        <v>621</v>
+      </c>
+      <c r="I1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="J1" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="K1" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="L1" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="M1" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="N1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="O1" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="P1" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="Q1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="93" t="s">
+      <c r="R1" s="93" t="s">
         <v>140</v>
       </c>
-      <c r="R1" s="95" t="s">
+      <c r="S1" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="T1" s="93" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="93" t="s">
+      <c r="U1" s="93" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="95" t="s">
+      <c r="V1" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="93" t="s">
+      <c r="W1" s="93" t="s">
         <v>143</v>
       </c>
-      <c r="W1" s="95" t="s">
+      <c r="X1" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="93" t="s">
+      <c r="Y1" s="93" t="s">
         <v>144</v>
       </c>
-      <c r="Y1" s="96" t="s">
+      <c r="Z1" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="Z1" s="62" t="s">
+      <c r="AA1" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="AA1" s="63" t="s">
+      <c r="AB1" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AC1" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="63" t="s">
+      <c r="AD1" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="63" t="s">
+      <c r="AE1" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="63" t="s">
+      <c r="AF1" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" s="63" t="s">
+      <c r="AG1" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="62" t="s">
+      <c r="AH1" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="AH1" s="62" t="s">
+      <c r="AI1" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="AI1" s="64" t="s">
+      <c r="AJ1" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="AJ1" s="97" t="s">
+      <c r="AK1" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="AK1" s="98" t="s">
+      <c r="AL1" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="AL1" s="63" t="s">
+      <c r="AM1" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="AM1" s="63" t="s">
+      <c r="AN1" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="AN1" s="63" t="s">
+      <c r="AO1" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="AO1" s="63" t="s">
+      <c r="AP1" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="AP1" s="62" t="s">
+      <c r="AQ1" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="AQ1" s="62" t="s">
+      <c r="AR1" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="AR1" s="62" t="s">
+      <c r="AS1" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="AS1" s="63" t="s">
+      <c r="AT1" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="AT1" s="63" t="s">
+      <c r="AU1" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="AU1" s="63" t="s">
+      <c r="AV1" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="AV1" s="63" t="s">
+      <c r="AW1" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="AW1" s="62" t="s">
+      <c r="AX1" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="AX1" s="62" t="s">
+      <c r="AY1" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="AY1" s="63" t="s">
+      <c r="AZ1" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" s="63" t="s">
+      <c r="BA1" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="BA1" s="63" t="s">
+      <c r="BB1" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="BB1" s="63" t="s">
+      <c r="BC1" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="BC1" s="62" t="s">
+      <c r="BD1" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="BD1" s="62" t="s">
+      <c r="BE1" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="BE1" s="63" t="s">
+      <c r="BF1" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="BF1" s="63" t="s">
+      <c r="BG1" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="BG1" s="63" t="s">
+      <c r="BH1" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="BH1" s="67" t="s">
+      <c r="BI1" s="67" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>179</v>
       </c>
@@ -24556,66 +24568,68 @@
         <v>2021</v>
       </c>
       <c r="G2" s="23">
-        <f>SUM(H2:I2,J2,M2)</f>
+        <f>SUM(I2:J2,K2,N2)</f>
         <v>357</v>
       </c>
       <c r="H2" s="23">
+        <v>268</v>
+      </c>
+      <c r="I2" s="23">
         <v>145</v>
       </c>
-      <c r="I2" s="23">
+      <c r="J2" s="23">
         <v>123</v>
       </c>
-      <c r="J2" s="23">
+      <c r="K2" s="23">
         <v>55</v>
       </c>
-      <c r="K2" s="23">
+      <c r="L2" s="23">
         <v>35</v>
       </c>
-      <c r="L2" s="23">
+      <c r="M2" s="23">
         <v>20</v>
       </c>
-      <c r="M2" s="23">
+      <c r="N2" s="23">
         <v>34</v>
       </c>
-      <c r="N2" s="23">
+      <c r="O2" s="23">
         <v>22</v>
       </c>
-      <c r="O2" s="23">
+      <c r="P2" s="23">
         <v>12</v>
       </c>
-      <c r="P2" s="23">
+      <c r="Q2" s="23">
         <v>8</v>
       </c>
-      <c r="Q2" s="23">
+      <c r="R2" s="23">
         <v>53</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="T2" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="23"/>
-      <c r="U2" s="22" t="s">
+      <c r="U2" s="23"/>
+      <c r="V2" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="V2" s="23"/>
-      <c r="W2" s="22" t="s">
+      <c r="W2" s="23"/>
+      <c r="X2" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="X2" s="23">
+      <c r="Y2" s="23">
         <v>2</v>
       </c>
-      <c r="Y2" s="23">
+      <c r="Z2" s="23">
         <v>600</v>
       </c>
-      <c r="Z2" s="23">
+      <c r="AA2" s="23">
         <v>100</v>
       </c>
-      <c r="AA2" s="23">
+      <c r="AB2" s="23">
         <v>30</v>
       </c>
-      <c r="AB2" s="74"/>
       <c r="AC2" s="74"/>
       <c r="AD2" s="74"/>
       <c r="AE2" s="74"/>
@@ -24624,46 +24638,46 @@
       <c r="AH2" s="74"/>
       <c r="AI2" s="74"/>
       <c r="AJ2" s="74"/>
-      <c r="AK2" s="23">
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="23">
         <v>15</v>
-      </c>
-      <c r="AL2" s="23">
-        <v>7</v>
       </c>
       <c r="AM2" s="23">
         <v>7</v>
       </c>
       <c r="AN2" s="23">
+        <v>7</v>
+      </c>
+      <c r="AO2" s="23">
         <v>1</v>
       </c>
-      <c r="AO2" s="23">
+      <c r="AP2" s="23">
         <v>0</v>
       </c>
-      <c r="AP2" s="22" t="s">
+      <c r="AQ2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="AQ2" s="22" t="s">
+      <c r="AR2" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="AR2" s="23">
+      <c r="AS2" s="23">
         <v>22</v>
       </c>
-      <c r="AS2" s="23">
+      <c r="AT2" s="23">
         <v>10</v>
       </c>
-      <c r="AT2" s="23">
+      <c r="AU2" s="23">
         <v>2</v>
-      </c>
-      <c r="AU2" s="23">
-        <v>5</v>
       </c>
       <c r="AV2" s="23">
         <v>5</v>
       </c>
-      <c r="AW2" s="22" t="s">
+      <c r="AW2" s="23">
+        <v>5</v>
+      </c>
+      <c r="AX2" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="AX2" s="74"/>
       <c r="AY2" s="74"/>
       <c r="AZ2" s="74"/>
       <c r="BA2" s="74"/>
@@ -24674,8 +24688,9 @@
       <c r="BF2" s="74"/>
       <c r="BG2" s="74"/>
       <c r="BH2" s="74"/>
-    </row>
-    <row r="3" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI2" s="74"/>
+    </row>
+    <row r="3" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74"/>
       <c r="B3" s="74"/>
       <c r="C3" s="22"/>
@@ -24695,10 +24710,10 @@
       <c r="Q3" s="74"/>
       <c r="R3" s="74"/>
       <c r="S3" s="74"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="74"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="23"/>
       <c r="X3" s="74"/>
       <c r="Y3" s="74"/>
       <c r="Z3" s="74"/>
@@ -24736,8 +24751,9 @@
       <c r="BF3" s="74"/>
       <c r="BG3" s="74"/>
       <c r="BH3" s="74"/>
-    </row>
-    <row r="4" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI3" s="74"/>
+    </row>
+    <row r="4" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74"/>
       <c r="B4" s="74"/>
       <c r="C4" s="22"/>
@@ -24757,10 +24773,10 @@
       <c r="Q4" s="74"/>
       <c r="R4" s="74"/>
       <c r="S4" s="74"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="74"/>
+      <c r="W4" s="23"/>
       <c r="X4" s="74"/>
       <c r="Y4" s="74"/>
       <c r="Z4" s="74"/>
@@ -24798,8 +24814,9 @@
       <c r="BF4" s="74"/>
       <c r="BG4" s="74"/>
       <c r="BH4" s="74"/>
-    </row>
-    <row r="5" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="74"/>
+    </row>
+    <row r="5" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
       <c r="B5" s="74"/>
       <c r="C5" s="22"/>
@@ -24819,10 +24836,10 @@
       <c r="Q5" s="74"/>
       <c r="R5" s="74"/>
       <c r="S5" s="74"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="23"/>
       <c r="X5" s="74"/>
       <c r="Y5" s="74"/>
       <c r="Z5" s="74"/>
@@ -24860,8 +24877,9 @@
       <c r="BF5" s="74"/>
       <c r="BG5" s="74"/>
       <c r="BH5" s="74"/>
-    </row>
-    <row r="6" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI5" s="74"/>
+    </row>
+    <row r="6" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="74"/>
       <c r="B6" s="74"/>
       <c r="C6" s="22"/>
@@ -24881,10 +24899,10 @@
       <c r="Q6" s="74"/>
       <c r="R6" s="74"/>
       <c r="S6" s="74"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="74"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="74"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="74"/>
+      <c r="W6" s="23"/>
       <c r="X6" s="74"/>
       <c r="Y6" s="74"/>
       <c r="Z6" s="74"/>
@@ -24922,8 +24940,9 @@
       <c r="BF6" s="74"/>
       <c r="BG6" s="74"/>
       <c r="BH6" s="74"/>
-    </row>
-    <row r="7" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI6" s="74"/>
+    </row>
+    <row r="7" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="74"/>
       <c r="B7" s="74"/>
       <c r="C7" s="22"/>
@@ -24943,10 +24962,10 @@
       <c r="Q7" s="74"/>
       <c r="R7" s="74"/>
       <c r="S7" s="74"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="74"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="23"/>
       <c r="X7" s="74"/>
       <c r="Y7" s="74"/>
       <c r="Z7" s="74"/>
@@ -24984,8 +25003,9 @@
       <c r="BF7" s="74"/>
       <c r="BG7" s="74"/>
       <c r="BH7" s="74"/>
-    </row>
-    <row r="8" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI7" s="74"/>
+    </row>
+    <row r="8" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="74"/>
       <c r="B8" s="74"/>
       <c r="C8" s="22"/>
@@ -25005,10 +25025,10 @@
       <c r="Q8" s="74"/>
       <c r="R8" s="74"/>
       <c r="S8" s="74"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="23"/>
       <c r="X8" s="74"/>
       <c r="Y8" s="74"/>
       <c r="Z8" s="74"/>
@@ -25046,8 +25066,9 @@
       <c r="BF8" s="74"/>
       <c r="BG8" s="74"/>
       <c r="BH8" s="74"/>
-    </row>
-    <row r="9" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI8" s="74"/>
+    </row>
+    <row r="9" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74"/>
       <c r="B9" s="74"/>
       <c r="C9" s="22"/>
@@ -25067,10 +25088,10 @@
       <c r="Q9" s="74"/>
       <c r="R9" s="74"/>
       <c r="S9" s="74"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="23"/>
-      <c r="W9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="23"/>
       <c r="X9" s="74"/>
       <c r="Y9" s="74"/>
       <c r="Z9" s="74"/>
@@ -25108,8 +25129,9 @@
       <c r="BF9" s="74"/>
       <c r="BG9" s="74"/>
       <c r="BH9" s="74"/>
-    </row>
-    <row r="10" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI9" s="74"/>
+    </row>
+    <row r="10" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="74"/>
       <c r="B10" s="74"/>
       <c r="C10" s="22"/>
@@ -25129,10 +25151,10 @@
       <c r="Q10" s="74"/>
       <c r="R10" s="74"/>
       <c r="S10" s="74"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="74"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="23"/>
       <c r="X10" s="74"/>
       <c r="Y10" s="74"/>
       <c r="Z10" s="74"/>
@@ -25170,8 +25192,9 @@
       <c r="BF10" s="74"/>
       <c r="BG10" s="74"/>
       <c r="BH10" s="74"/>
-    </row>
-    <row r="11" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI10" s="74"/>
+    </row>
+    <row r="11" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="74"/>
       <c r="B11" s="74"/>
       <c r="C11" s="22"/>
@@ -25191,10 +25214,10 @@
       <c r="Q11" s="74"/>
       <c r="R11" s="74"/>
       <c r="S11" s="74"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="74"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="74"/>
+      <c r="T11" s="74"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="74"/>
+      <c r="W11" s="23"/>
       <c r="X11" s="74"/>
       <c r="Y11" s="74"/>
       <c r="Z11" s="74"/>
@@ -25232,8 +25255,9 @@
       <c r="BF11" s="74"/>
       <c r="BG11" s="74"/>
       <c r="BH11" s="74"/>
-    </row>
-    <row r="12" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI11" s="74"/>
+    </row>
+    <row r="12" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74"/>
       <c r="B12" s="74"/>
       <c r="C12" s="22"/>
@@ -25253,10 +25277,10 @@
       <c r="Q12" s="74"/>
       <c r="R12" s="74"/>
       <c r="S12" s="74"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="74"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="74"/>
+      <c r="T12" s="74"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="23"/>
       <c r="X12" s="74"/>
       <c r="Y12" s="74"/>
       <c r="Z12" s="74"/>
@@ -25294,8 +25318,9 @@
       <c r="BF12" s="74"/>
       <c r="BG12" s="74"/>
       <c r="BH12" s="74"/>
-    </row>
-    <row r="13" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI12" s="74"/>
+    </row>
+    <row r="13" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
       <c r="B13" s="74"/>
       <c r="C13" s="22"/>
@@ -25315,10 +25340,10 @@
       <c r="Q13" s="74"/>
       <c r="R13" s="74"/>
       <c r="S13" s="74"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="74"/>
-      <c r="V13" s="23"/>
-      <c r="W13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="23"/>
       <c r="X13" s="74"/>
       <c r="Y13" s="74"/>
       <c r="Z13" s="74"/>
@@ -25356,8 +25381,9 @@
       <c r="BF13" s="74"/>
       <c r="BG13" s="74"/>
       <c r="BH13" s="74"/>
-    </row>
-    <row r="14" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI13" s="74"/>
+    </row>
+    <row r="14" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="74"/>
       <c r="C14" s="22"/>
@@ -25377,10 +25403,10 @@
       <c r="Q14" s="74"/>
       <c r="R14" s="74"/>
       <c r="S14" s="74"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="74"/>
-      <c r="V14" s="23"/>
-      <c r="W14" s="74"/>
+      <c r="T14" s="74"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="74"/>
+      <c r="W14" s="23"/>
       <c r="X14" s="74"/>
       <c r="Y14" s="74"/>
       <c r="Z14" s="74"/>
@@ -25418,8 +25444,9 @@
       <c r="BF14" s="74"/>
       <c r="BG14" s="74"/>
       <c r="BH14" s="74"/>
-    </row>
-    <row r="15" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI14" s="74"/>
+    </row>
+    <row r="15" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="74"/>
       <c r="C15" s="22"/>
@@ -25439,10 +25466,10 @@
       <c r="Q15" s="74"/>
       <c r="R15" s="74"/>
       <c r="S15" s="74"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="74"/>
-      <c r="V15" s="23"/>
-      <c r="W15" s="74"/>
+      <c r="T15" s="74"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="74"/>
+      <c r="W15" s="23"/>
       <c r="X15" s="74"/>
       <c r="Y15" s="74"/>
       <c r="Z15" s="74"/>
@@ -25480,8 +25507,9 @@
       <c r="BF15" s="74"/>
       <c r="BG15" s="74"/>
       <c r="BH15" s="74"/>
-    </row>
-    <row r="16" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI15" s="74"/>
+    </row>
+    <row r="16" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="74"/>
       <c r="C16" s="22"/>
@@ -25501,10 +25529,10 @@
       <c r="Q16" s="74"/>
       <c r="R16" s="74"/>
       <c r="S16" s="74"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="74"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="74"/>
+      <c r="W16" s="23"/>
       <c r="X16" s="74"/>
       <c r="Y16" s="74"/>
       <c r="Z16" s="74"/>
@@ -25542,8 +25570,9 @@
       <c r="BF16" s="74"/>
       <c r="BG16" s="74"/>
       <c r="BH16" s="74"/>
-    </row>
-    <row r="17" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI16" s="74"/>
+    </row>
+    <row r="17" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
       <c r="B17" s="74"/>
       <c r="C17" s="22"/>
@@ -25563,10 +25592,10 @@
       <c r="Q17" s="74"/>
       <c r="R17" s="74"/>
       <c r="S17" s="74"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="74"/>
-      <c r="V17" s="23"/>
-      <c r="W17" s="74"/>
+      <c r="T17" s="74"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="74"/>
+      <c r="W17" s="23"/>
       <c r="X17" s="74"/>
       <c r="Y17" s="74"/>
       <c r="Z17" s="74"/>
@@ -25604,8 +25633,9 @@
       <c r="BF17" s="74"/>
       <c r="BG17" s="74"/>
       <c r="BH17" s="74"/>
-    </row>
-    <row r="18" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI17" s="74"/>
+    </row>
+    <row r="18" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="74"/>
       <c r="C18" s="22"/>
@@ -25625,10 +25655,10 @@
       <c r="Q18" s="74"/>
       <c r="R18" s="74"/>
       <c r="S18" s="74"/>
-      <c r="T18" s="23"/>
-      <c r="U18" s="74"/>
-      <c r="V18" s="23"/>
-      <c r="W18" s="74"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="74"/>
+      <c r="W18" s="23"/>
       <c r="X18" s="74"/>
       <c r="Y18" s="74"/>
       <c r="Z18" s="74"/>
@@ -25666,8 +25696,9 @@
       <c r="BF18" s="74"/>
       <c r="BG18" s="74"/>
       <c r="BH18" s="74"/>
-    </row>
-    <row r="19" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI18" s="74"/>
+    </row>
+    <row r="19" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
       <c r="B19" s="74"/>
       <c r="C19" s="22"/>
@@ -25687,10 +25718,10 @@
       <c r="Q19" s="74"/>
       <c r="R19" s="74"/>
       <c r="S19" s="74"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="74"/>
+      <c r="W19" s="23"/>
       <c r="X19" s="74"/>
       <c r="Y19" s="74"/>
       <c r="Z19" s="74"/>
@@ -25728,8 +25759,9 @@
       <c r="BF19" s="74"/>
       <c r="BG19" s="74"/>
       <c r="BH19" s="74"/>
-    </row>
-    <row r="20" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI19" s="74"/>
+    </row>
+    <row r="20" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
       <c r="B20" s="74"/>
       <c r="C20" s="22"/>
@@ -25749,10 +25781,10 @@
       <c r="Q20" s="74"/>
       <c r="R20" s="74"/>
       <c r="S20" s="74"/>
-      <c r="T20" s="23"/>
-      <c r="U20" s="74"/>
-      <c r="V20" s="23"/>
-      <c r="W20" s="74"/>
+      <c r="T20" s="74"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="74"/>
+      <c r="W20" s="23"/>
       <c r="X20" s="74"/>
       <c r="Y20" s="74"/>
       <c r="Z20" s="74"/>
@@ -25790,8 +25822,9 @@
       <c r="BF20" s="74"/>
       <c r="BG20" s="74"/>
       <c r="BH20" s="74"/>
-    </row>
-    <row r="21" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI20" s="74"/>
+    </row>
+    <row r="21" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="74"/>
       <c r="C21" s="22"/>
@@ -25811,10 +25844,10 @@
       <c r="Q21" s="74"/>
       <c r="R21" s="74"/>
       <c r="S21" s="74"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="74"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="74"/>
+      <c r="T21" s="74"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="74"/>
+      <c r="W21" s="23"/>
       <c r="X21" s="74"/>
       <c r="Y21" s="74"/>
       <c r="Z21" s="74"/>
@@ -25852,8 +25885,9 @@
       <c r="BF21" s="74"/>
       <c r="BG21" s="74"/>
       <c r="BH21" s="74"/>
-    </row>
-    <row r="22" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI21" s="74"/>
+    </row>
+    <row r="22" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="74"/>
       <c r="B22" s="74"/>
       <c r="C22" s="22"/>
@@ -25873,10 +25907,10 @@
       <c r="Q22" s="74"/>
       <c r="R22" s="74"/>
       <c r="S22" s="74"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="74"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="74"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="74"/>
+      <c r="W22" s="23"/>
       <c r="X22" s="74"/>
       <c r="Y22" s="74"/>
       <c r="Z22" s="74"/>
@@ -25914,8 +25948,9 @@
       <c r="BF22" s="74"/>
       <c r="BG22" s="74"/>
       <c r="BH22" s="74"/>
-    </row>
-    <row r="23" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI22" s="74"/>
+    </row>
+    <row r="23" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="74"/>
       <c r="B23" s="74"/>
       <c r="C23" s="22"/>
@@ -25935,10 +25970,10 @@
       <c r="Q23" s="74"/>
       <c r="R23" s="74"/>
       <c r="S23" s="74"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="74"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="74"/>
+      <c r="T23" s="74"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="74"/>
+      <c r="W23" s="23"/>
       <c r="X23" s="74"/>
       <c r="Y23" s="74"/>
       <c r="Z23" s="74"/>
@@ -25976,8 +26011,9 @@
       <c r="BF23" s="74"/>
       <c r="BG23" s="74"/>
       <c r="BH23" s="74"/>
-    </row>
-    <row r="24" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI23" s="74"/>
+    </row>
+    <row r="24" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="74"/>
       <c r="B24" s="74"/>
       <c r="C24" s="22"/>
@@ -25997,10 +26033,10 @@
       <c r="Q24" s="74"/>
       <c r="R24" s="74"/>
       <c r="S24" s="74"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="74"/>
-      <c r="V24" s="23"/>
-      <c r="W24" s="74"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="74"/>
+      <c r="W24" s="23"/>
       <c r="X24" s="74"/>
       <c r="Y24" s="74"/>
       <c r="Z24" s="74"/>
@@ -26038,8 +26074,9 @@
       <c r="BF24" s="74"/>
       <c r="BG24" s="74"/>
       <c r="BH24" s="74"/>
-    </row>
-    <row r="25" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI24" s="74"/>
+    </row>
+    <row r="25" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="74"/>
       <c r="B25" s="74"/>
       <c r="C25" s="22"/>
@@ -26059,10 +26096,10 @@
       <c r="Q25" s="74"/>
       <c r="R25" s="74"/>
       <c r="S25" s="74"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="74"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="74"/>
+      <c r="T25" s="74"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="74"/>
+      <c r="W25" s="23"/>
       <c r="X25" s="74"/>
       <c r="Y25" s="74"/>
       <c r="Z25" s="74"/>
@@ -26100,8 +26137,9 @@
       <c r="BF25" s="74"/>
       <c r="BG25" s="74"/>
       <c r="BH25" s="74"/>
-    </row>
-    <row r="26" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI25" s="74"/>
+    </row>
+    <row r="26" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="74"/>
       <c r="B26" s="74"/>
       <c r="C26" s="22"/>
@@ -26121,10 +26159,10 @@
       <c r="Q26" s="74"/>
       <c r="R26" s="74"/>
       <c r="S26" s="74"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="74"/>
-      <c r="V26" s="23"/>
-      <c r="W26" s="74"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="23"/>
       <c r="X26" s="74"/>
       <c r="Y26" s="74"/>
       <c r="Z26" s="74"/>
@@ -26162,8 +26200,9 @@
       <c r="BF26" s="74"/>
       <c r="BG26" s="74"/>
       <c r="BH26" s="74"/>
-    </row>
-    <row r="27" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI26" s="74"/>
+    </row>
+    <row r="27" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="74"/>
       <c r="B27" s="74"/>
       <c r="C27" s="22"/>
@@ -26183,10 +26222,10 @@
       <c r="Q27" s="74"/>
       <c r="R27" s="74"/>
       <c r="S27" s="74"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="74"/>
-      <c r="V27" s="23"/>
-      <c r="W27" s="74"/>
+      <c r="T27" s="74"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="23"/>
       <c r="X27" s="74"/>
       <c r="Y27" s="74"/>
       <c r="Z27" s="74"/>
@@ -26224,8 +26263,9 @@
       <c r="BF27" s="74"/>
       <c r="BG27" s="74"/>
       <c r="BH27" s="74"/>
-    </row>
-    <row r="28" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI27" s="74"/>
+    </row>
+    <row r="28" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="74"/>
       <c r="B28" s="74"/>
       <c r="C28" s="22"/>
@@ -26245,10 +26285,10 @@
       <c r="Q28" s="74"/>
       <c r="R28" s="74"/>
       <c r="S28" s="74"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="74"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="74"/>
+      <c r="T28" s="74"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="23"/>
       <c r="X28" s="74"/>
       <c r="Y28" s="74"/>
       <c r="Z28" s="74"/>
@@ -26286,8 +26326,9 @@
       <c r="BF28" s="74"/>
       <c r="BG28" s="74"/>
       <c r="BH28" s="74"/>
-    </row>
-    <row r="29" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI28" s="74"/>
+    </row>
+    <row r="29" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="74"/>
       <c r="B29" s="74"/>
       <c r="C29" s="22"/>
@@ -26307,10 +26348,10 @@
       <c r="Q29" s="74"/>
       <c r="R29" s="74"/>
       <c r="S29" s="74"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="74"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="74"/>
+      <c r="T29" s="74"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="23"/>
       <c r="X29" s="74"/>
       <c r="Y29" s="74"/>
       <c r="Z29" s="74"/>
@@ -26348,8 +26389,9 @@
       <c r="BF29" s="74"/>
       <c r="BG29" s="74"/>
       <c r="BH29" s="74"/>
-    </row>
-    <row r="30" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI29" s="74"/>
+    </row>
+    <row r="30" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="74"/>
       <c r="B30" s="74"/>
       <c r="C30" s="22"/>
@@ -26369,10 +26411,10 @@
       <c r="Q30" s="74"/>
       <c r="R30" s="74"/>
       <c r="S30" s="74"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="74"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="74"/>
+      <c r="T30" s="74"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="23"/>
       <c r="X30" s="74"/>
       <c r="Y30" s="74"/>
       <c r="Z30" s="74"/>
@@ -26410,8 +26452,9 @@
       <c r="BF30" s="74"/>
       <c r="BG30" s="74"/>
       <c r="BH30" s="74"/>
-    </row>
-    <row r="31" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI30" s="74"/>
+    </row>
+    <row r="31" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="74"/>
       <c r="B31" s="74"/>
       <c r="C31" s="22"/>
@@ -26431,10 +26474,10 @@
       <c r="Q31" s="74"/>
       <c r="R31" s="74"/>
       <c r="S31" s="74"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="74"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="74"/>
+      <c r="T31" s="74"/>
+      <c r="U31" s="23"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="23"/>
       <c r="X31" s="74"/>
       <c r="Y31" s="74"/>
       <c r="Z31" s="74"/>
@@ -26472,8 +26515,9 @@
       <c r="BF31" s="74"/>
       <c r="BG31" s="74"/>
       <c r="BH31" s="74"/>
-    </row>
-    <row r="32" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI31" s="74"/>
+    </row>
+    <row r="32" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="74"/>
       <c r="B32" s="74"/>
       <c r="C32" s="22"/>
@@ -26493,10 +26537,10 @@
       <c r="Q32" s="74"/>
       <c r="R32" s="74"/>
       <c r="S32" s="74"/>
-      <c r="T32" s="23"/>
-      <c r="U32" s="74"/>
-      <c r="V32" s="23"/>
-      <c r="W32" s="74"/>
+      <c r="T32" s="74"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="23"/>
       <c r="X32" s="74"/>
       <c r="Y32" s="74"/>
       <c r="Z32" s="74"/>
@@ -26534,8 +26578,9 @@
       <c r="BF32" s="74"/>
       <c r="BG32" s="74"/>
       <c r="BH32" s="74"/>
-    </row>
-    <row r="33" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI32" s="74"/>
+    </row>
+    <row r="33" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="74"/>
       <c r="B33" s="74"/>
       <c r="C33" s="22"/>
@@ -26555,10 +26600,10 @@
       <c r="Q33" s="74"/>
       <c r="R33" s="74"/>
       <c r="S33" s="74"/>
-      <c r="T33" s="23"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="23"/>
-      <c r="W33" s="74"/>
+      <c r="T33" s="74"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="23"/>
       <c r="X33" s="74"/>
       <c r="Y33" s="74"/>
       <c r="Z33" s="74"/>
@@ -26596,8 +26641,9 @@
       <c r="BF33" s="74"/>
       <c r="BG33" s="74"/>
       <c r="BH33" s="74"/>
-    </row>
-    <row r="34" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI33" s="74"/>
+    </row>
+    <row r="34" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74"/>
       <c r="B34" s="74"/>
       <c r="C34" s="22"/>
@@ -26617,10 +26663,10 @@
       <c r="Q34" s="74"/>
       <c r="R34" s="74"/>
       <c r="S34" s="74"/>
-      <c r="T34" s="23"/>
-      <c r="U34" s="74"/>
-      <c r="V34" s="23"/>
-      <c r="W34" s="74"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="23"/>
       <c r="X34" s="74"/>
       <c r="Y34" s="74"/>
       <c r="Z34" s="74"/>
@@ -26658,8 +26704,9 @@
       <c r="BF34" s="74"/>
       <c r="BG34" s="74"/>
       <c r="BH34" s="74"/>
-    </row>
-    <row r="35" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI34" s="74"/>
+    </row>
+    <row r="35" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="74"/>
       <c r="B35" s="74"/>
       <c r="C35" s="22"/>
@@ -26679,10 +26726,10 @@
       <c r="Q35" s="74"/>
       <c r="R35" s="74"/>
       <c r="S35" s="74"/>
-      <c r="T35" s="23"/>
-      <c r="U35" s="74"/>
-      <c r="V35" s="23"/>
-      <c r="W35" s="74"/>
+      <c r="T35" s="74"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="74"/>
+      <c r="W35" s="23"/>
       <c r="X35" s="74"/>
       <c r="Y35" s="74"/>
       <c r="Z35" s="74"/>
@@ -26720,8 +26767,9 @@
       <c r="BF35" s="74"/>
       <c r="BG35" s="74"/>
       <c r="BH35" s="74"/>
-    </row>
-    <row r="36" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI35" s="74"/>
+    </row>
+    <row r="36" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="74"/>
       <c r="B36" s="74"/>
       <c r="C36" s="22"/>
@@ -26741,10 +26789,10 @@
       <c r="Q36" s="74"/>
       <c r="R36" s="74"/>
       <c r="S36" s="74"/>
-      <c r="T36" s="23"/>
-      <c r="U36" s="74"/>
-      <c r="V36" s="23"/>
-      <c r="W36" s="74"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="23"/>
       <c r="X36" s="74"/>
       <c r="Y36" s="74"/>
       <c r="Z36" s="74"/>
@@ -26782,8 +26830,9 @@
       <c r="BF36" s="74"/>
       <c r="BG36" s="74"/>
       <c r="BH36" s="74"/>
-    </row>
-    <row r="37" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI36" s="74"/>
+    </row>
+    <row r="37" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="74"/>
       <c r="B37" s="74"/>
       <c r="C37" s="22"/>
@@ -26803,10 +26852,10 @@
       <c r="Q37" s="74"/>
       <c r="R37" s="74"/>
       <c r="S37" s="74"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="74"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="74"/>
+      <c r="T37" s="74"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="23"/>
       <c r="X37" s="74"/>
       <c r="Y37" s="74"/>
       <c r="Z37" s="74"/>
@@ -26844,8 +26893,9 @@
       <c r="BF37" s="74"/>
       <c r="BG37" s="74"/>
       <c r="BH37" s="74"/>
-    </row>
-    <row r="38" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI37" s="74"/>
+    </row>
+    <row r="38" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="74"/>
       <c r="B38" s="74"/>
       <c r="C38" s="22"/>
@@ -26865,10 +26915,10 @@
       <c r="Q38" s="74"/>
       <c r="R38" s="74"/>
       <c r="S38" s="74"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="74"/>
-      <c r="V38" s="23"/>
-      <c r="W38" s="74"/>
+      <c r="T38" s="74"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="23"/>
       <c r="X38" s="74"/>
       <c r="Y38" s="74"/>
       <c r="Z38" s="74"/>
@@ -26906,8 +26956,9 @@
       <c r="BF38" s="74"/>
       <c r="BG38" s="74"/>
       <c r="BH38" s="74"/>
-    </row>
-    <row r="39" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI38" s="74"/>
+    </row>
+    <row r="39" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="74"/>
       <c r="B39" s="74"/>
       <c r="C39" s="22"/>
@@ -26927,10 +26978,10 @@
       <c r="Q39" s="74"/>
       <c r="R39" s="74"/>
       <c r="S39" s="74"/>
-      <c r="T39" s="23"/>
-      <c r="U39" s="74"/>
-      <c r="V39" s="23"/>
-      <c r="W39" s="74"/>
+      <c r="T39" s="74"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="23"/>
       <c r="X39" s="74"/>
       <c r="Y39" s="74"/>
       <c r="Z39" s="74"/>
@@ -26968,8 +27019,9 @@
       <c r="BF39" s="74"/>
       <c r="BG39" s="74"/>
       <c r="BH39" s="74"/>
-    </row>
-    <row r="40" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI39" s="74"/>
+    </row>
+    <row r="40" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="74"/>
       <c r="B40" s="74"/>
       <c r="C40" s="22"/>
@@ -26989,10 +27041,10 @@
       <c r="Q40" s="74"/>
       <c r="R40" s="74"/>
       <c r="S40" s="74"/>
-      <c r="T40" s="23"/>
-      <c r="U40" s="74"/>
-      <c r="V40" s="23"/>
-      <c r="W40" s="74"/>
+      <c r="T40" s="74"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="23"/>
       <c r="X40" s="74"/>
       <c r="Y40" s="74"/>
       <c r="Z40" s="74"/>
@@ -27030,8 +27082,9 @@
       <c r="BF40" s="74"/>
       <c r="BG40" s="74"/>
       <c r="BH40" s="74"/>
-    </row>
-    <row r="41" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI40" s="74"/>
+    </row>
+    <row r="41" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="74"/>
       <c r="B41" s="74"/>
       <c r="C41" s="22"/>
@@ -27051,10 +27104,10 @@
       <c r="Q41" s="74"/>
       <c r="R41" s="74"/>
       <c r="S41" s="74"/>
-      <c r="T41" s="23"/>
-      <c r="U41" s="74"/>
-      <c r="V41" s="23"/>
-      <c r="W41" s="74"/>
+      <c r="T41" s="74"/>
+      <c r="U41" s="23"/>
+      <c r="V41" s="74"/>
+      <c r="W41" s="23"/>
       <c r="X41" s="74"/>
       <c r="Y41" s="74"/>
       <c r="Z41" s="74"/>
@@ -27092,8 +27145,9 @@
       <c r="BF41" s="74"/>
       <c r="BG41" s="74"/>
       <c r="BH41" s="74"/>
-    </row>
-    <row r="42" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI41" s="74"/>
+    </row>
+    <row r="42" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="74"/>
       <c r="B42" s="74"/>
       <c r="C42" s="22"/>
@@ -27113,10 +27167,10 @@
       <c r="Q42" s="74"/>
       <c r="R42" s="74"/>
       <c r="S42" s="74"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="74"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="74"/>
+      <c r="T42" s="74"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="74"/>
+      <c r="W42" s="23"/>
       <c r="X42" s="74"/>
       <c r="Y42" s="74"/>
       <c r="Z42" s="74"/>
@@ -27154,8 +27208,9 @@
       <c r="BF42" s="74"/>
       <c r="BG42" s="74"/>
       <c r="BH42" s="74"/>
-    </row>
-    <row r="43" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI42" s="74"/>
+    </row>
+    <row r="43" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="74"/>
       <c r="B43" s="74"/>
       <c r="C43" s="22"/>
@@ -27175,10 +27230,10 @@
       <c r="Q43" s="74"/>
       <c r="R43" s="74"/>
       <c r="S43" s="74"/>
-      <c r="T43" s="23"/>
-      <c r="U43" s="74"/>
-      <c r="V43" s="23"/>
-      <c r="W43" s="74"/>
+      <c r="T43" s="74"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="74"/>
+      <c r="W43" s="23"/>
       <c r="X43" s="74"/>
       <c r="Y43" s="74"/>
       <c r="Z43" s="74"/>
@@ -27216,8 +27271,9 @@
       <c r="BF43" s="74"/>
       <c r="BG43" s="74"/>
       <c r="BH43" s="74"/>
-    </row>
-    <row r="44" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI43" s="74"/>
+    </row>
+    <row r="44" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="74"/>
       <c r="B44" s="74"/>
       <c r="C44" s="22"/>
@@ -27237,10 +27293,10 @@
       <c r="Q44" s="74"/>
       <c r="R44" s="74"/>
       <c r="S44" s="74"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="74"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="74"/>
+      <c r="T44" s="74"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="74"/>
+      <c r="W44" s="23"/>
       <c r="X44" s="74"/>
       <c r="Y44" s="74"/>
       <c r="Z44" s="74"/>
@@ -27278,8 +27334,9 @@
       <c r="BF44" s="74"/>
       <c r="BG44" s="74"/>
       <c r="BH44" s="74"/>
-    </row>
-    <row r="45" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI44" s="74"/>
+    </row>
+    <row r="45" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="74"/>
       <c r="B45" s="74"/>
       <c r="C45" s="22"/>
@@ -27299,10 +27356,10 @@
       <c r="Q45" s="74"/>
       <c r="R45" s="74"/>
       <c r="S45" s="74"/>
-      <c r="T45" s="23"/>
-      <c r="U45" s="74"/>
-      <c r="V45" s="23"/>
-      <c r="W45" s="74"/>
+      <c r="T45" s="74"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="23"/>
       <c r="X45" s="74"/>
       <c r="Y45" s="74"/>
       <c r="Z45" s="74"/>
@@ -27340,8 +27397,9 @@
       <c r="BF45" s="74"/>
       <c r="BG45" s="74"/>
       <c r="BH45" s="74"/>
-    </row>
-    <row r="46" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI45" s="74"/>
+    </row>
+    <row r="46" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="74"/>
       <c r="B46" s="74"/>
       <c r="C46" s="22"/>
@@ -27361,10 +27419,10 @@
       <c r="Q46" s="74"/>
       <c r="R46" s="74"/>
       <c r="S46" s="74"/>
-      <c r="T46" s="23"/>
-      <c r="U46" s="74"/>
-      <c r="V46" s="23"/>
-      <c r="W46" s="74"/>
+      <c r="T46" s="74"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="74"/>
+      <c r="W46" s="23"/>
       <c r="X46" s="74"/>
       <c r="Y46" s="74"/>
       <c r="Z46" s="74"/>
@@ -27402,8 +27460,9 @@
       <c r="BF46" s="74"/>
       <c r="BG46" s="74"/>
       <c r="BH46" s="74"/>
-    </row>
-    <row r="47" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI46" s="74"/>
+    </row>
+    <row r="47" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="74"/>
       <c r="B47" s="74"/>
       <c r="C47" s="22"/>
@@ -27423,10 +27482,10 @@
       <c r="Q47" s="74"/>
       <c r="R47" s="74"/>
       <c r="S47" s="74"/>
-      <c r="T47" s="23"/>
-      <c r="U47" s="74"/>
-      <c r="V47" s="23"/>
-      <c r="W47" s="74"/>
+      <c r="T47" s="74"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="74"/>
+      <c r="W47" s="23"/>
       <c r="X47" s="74"/>
       <c r="Y47" s="74"/>
       <c r="Z47" s="74"/>
@@ -27464,8 +27523,9 @@
       <c r="BF47" s="74"/>
       <c r="BG47" s="74"/>
       <c r="BH47" s="74"/>
-    </row>
-    <row r="48" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI47" s="74"/>
+    </row>
+    <row r="48" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="74"/>
       <c r="B48" s="74"/>
       <c r="C48" s="22"/>
@@ -27485,10 +27545,10 @@
       <c r="Q48" s="74"/>
       <c r="R48" s="74"/>
       <c r="S48" s="74"/>
-      <c r="T48" s="23"/>
-      <c r="U48" s="74"/>
-      <c r="V48" s="23"/>
-      <c r="W48" s="74"/>
+      <c r="T48" s="74"/>
+      <c r="U48" s="23"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="23"/>
       <c r="X48" s="74"/>
       <c r="Y48" s="74"/>
       <c r="Z48" s="74"/>
@@ -27526,8 +27586,9 @@
       <c r="BF48" s="74"/>
       <c r="BG48" s="74"/>
       <c r="BH48" s="74"/>
-    </row>
-    <row r="49" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI48" s="74"/>
+    </row>
+    <row r="49" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="74"/>
       <c r="B49" s="74"/>
       <c r="C49" s="22"/>
@@ -27547,10 +27608,10 @@
       <c r="Q49" s="74"/>
       <c r="R49" s="74"/>
       <c r="S49" s="74"/>
-      <c r="T49" s="23"/>
-      <c r="U49" s="74"/>
-      <c r="V49" s="23"/>
-      <c r="W49" s="74"/>
+      <c r="T49" s="74"/>
+      <c r="U49" s="23"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="23"/>
       <c r="X49" s="74"/>
       <c r="Y49" s="74"/>
       <c r="Z49" s="74"/>
@@ -27588,8 +27649,9 @@
       <c r="BF49" s="74"/>
       <c r="BG49" s="74"/>
       <c r="BH49" s="74"/>
-    </row>
-    <row r="50" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI49" s="74"/>
+    </row>
+    <row r="50" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="74"/>
       <c r="B50" s="74"/>
       <c r="C50" s="22"/>
@@ -27609,10 +27671,10 @@
       <c r="Q50" s="74"/>
       <c r="R50" s="74"/>
       <c r="S50" s="74"/>
-      <c r="T50" s="23"/>
-      <c r="U50" s="74"/>
-      <c r="V50" s="23"/>
-      <c r="W50" s="74"/>
+      <c r="T50" s="74"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="23"/>
       <c r="X50" s="74"/>
       <c r="Y50" s="74"/>
       <c r="Z50" s="74"/>
@@ -27650,8 +27712,9 @@
       <c r="BF50" s="74"/>
       <c r="BG50" s="74"/>
       <c r="BH50" s="74"/>
-    </row>
-    <row r="51" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI50" s="74"/>
+    </row>
+    <row r="51" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="74"/>
       <c r="B51" s="74"/>
       <c r="C51" s="22"/>
@@ -27671,10 +27734,10 @@
       <c r="Q51" s="74"/>
       <c r="R51" s="74"/>
       <c r="S51" s="74"/>
-      <c r="T51" s="23"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="23"/>
-      <c r="W51" s="74"/>
+      <c r="T51" s="74"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="74"/>
+      <c r="W51" s="23"/>
       <c r="X51" s="74"/>
       <c r="Y51" s="74"/>
       <c r="Z51" s="74"/>
@@ -27712,8 +27775,9 @@
       <c r="BF51" s="74"/>
       <c r="BG51" s="74"/>
       <c r="BH51" s="74"/>
-    </row>
-    <row r="52" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI51" s="74"/>
+    </row>
+    <row r="52" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="74"/>
       <c r="B52" s="74"/>
       <c r="C52" s="22"/>
@@ -27733,10 +27797,10 @@
       <c r="Q52" s="74"/>
       <c r="R52" s="74"/>
       <c r="S52" s="74"/>
-      <c r="T52" s="23"/>
-      <c r="U52" s="74"/>
-      <c r="V52" s="23"/>
-      <c r="W52" s="74"/>
+      <c r="T52" s="74"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="74"/>
+      <c r="W52" s="23"/>
       <c r="X52" s="74"/>
       <c r="Y52" s="74"/>
       <c r="Z52" s="74"/>
@@ -27774,8 +27838,9 @@
       <c r="BF52" s="74"/>
       <c r="BG52" s="74"/>
       <c r="BH52" s="74"/>
-    </row>
-    <row r="53" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI52" s="74"/>
+    </row>
+    <row r="53" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="74"/>
       <c r="B53" s="74"/>
       <c r="C53" s="22"/>
@@ -27795,10 +27860,10 @@
       <c r="Q53" s="74"/>
       <c r="R53" s="74"/>
       <c r="S53" s="74"/>
-      <c r="T53" s="23"/>
-      <c r="U53" s="74"/>
-      <c r="V53" s="23"/>
-      <c r="W53" s="74"/>
+      <c r="T53" s="74"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="74"/>
+      <c r="W53" s="23"/>
       <c r="X53" s="74"/>
       <c r="Y53" s="74"/>
       <c r="Z53" s="74"/>
@@ -27836,8 +27901,9 @@
       <c r="BF53" s="74"/>
       <c r="BG53" s="74"/>
       <c r="BH53" s="74"/>
-    </row>
-    <row r="54" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI53" s="74"/>
+    </row>
+    <row r="54" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="74"/>
       <c r="B54" s="74"/>
       <c r="C54" s="22"/>
@@ -27857,10 +27923,10 @@
       <c r="Q54" s="74"/>
       <c r="R54" s="74"/>
       <c r="S54" s="74"/>
-      <c r="T54" s="23"/>
-      <c r="U54" s="74"/>
-      <c r="V54" s="23"/>
-      <c r="W54" s="74"/>
+      <c r="T54" s="74"/>
+      <c r="U54" s="23"/>
+      <c r="V54" s="74"/>
+      <c r="W54" s="23"/>
       <c r="X54" s="74"/>
       <c r="Y54" s="74"/>
       <c r="Z54" s="74"/>
@@ -27898,8 +27964,9 @@
       <c r="BF54" s="74"/>
       <c r="BG54" s="74"/>
       <c r="BH54" s="74"/>
-    </row>
-    <row r="55" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI54" s="74"/>
+    </row>
+    <row r="55" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="74"/>
       <c r="B55" s="74"/>
       <c r="C55" s="22"/>
@@ -27919,10 +27986,10 @@
       <c r="Q55" s="74"/>
       <c r="R55" s="74"/>
       <c r="S55" s="74"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="74"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="74"/>
+      <c r="T55" s="74"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="74"/>
+      <c r="W55" s="23"/>
       <c r="X55" s="74"/>
       <c r="Y55" s="74"/>
       <c r="Z55" s="74"/>
@@ -27960,8 +28027,9 @@
       <c r="BF55" s="74"/>
       <c r="BG55" s="74"/>
       <c r="BH55" s="74"/>
-    </row>
-    <row r="56" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI55" s="74"/>
+    </row>
+    <row r="56" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="74"/>
       <c r="B56" s="74"/>
       <c r="C56" s="22"/>
@@ -27981,10 +28049,10 @@
       <c r="Q56" s="74"/>
       <c r="R56" s="74"/>
       <c r="S56" s="74"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="74"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="74"/>
+      <c r="T56" s="74"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="74"/>
+      <c r="W56" s="23"/>
       <c r="X56" s="74"/>
       <c r="Y56" s="74"/>
       <c r="Z56" s="74"/>
@@ -28022,8 +28090,9 @@
       <c r="BF56" s="74"/>
       <c r="BG56" s="74"/>
       <c r="BH56" s="74"/>
-    </row>
-    <row r="57" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI56" s="74"/>
+    </row>
+    <row r="57" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="74"/>
       <c r="B57" s="74"/>
       <c r="C57" s="22"/>
@@ -28043,10 +28112,10 @@
       <c r="Q57" s="74"/>
       <c r="R57" s="74"/>
       <c r="S57" s="74"/>
-      <c r="T57" s="23"/>
-      <c r="U57" s="74"/>
-      <c r="V57" s="23"/>
-      <c r="W57" s="74"/>
+      <c r="T57" s="74"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="74"/>
+      <c r="W57" s="23"/>
       <c r="X57" s="74"/>
       <c r="Y57" s="74"/>
       <c r="Z57" s="74"/>
@@ -28084,8 +28153,9 @@
       <c r="BF57" s="74"/>
       <c r="BG57" s="74"/>
       <c r="BH57" s="74"/>
-    </row>
-    <row r="58" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI57" s="74"/>
+    </row>
+    <row r="58" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="74"/>
       <c r="B58" s="74"/>
       <c r="C58" s="22"/>
@@ -28105,10 +28175,10 @@
       <c r="Q58" s="74"/>
       <c r="R58" s="74"/>
       <c r="S58" s="74"/>
-      <c r="T58" s="23"/>
-      <c r="U58" s="74"/>
-      <c r="V58" s="23"/>
-      <c r="W58" s="74"/>
+      <c r="T58" s="74"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="74"/>
+      <c r="W58" s="23"/>
       <c r="X58" s="74"/>
       <c r="Y58" s="74"/>
       <c r="Z58" s="74"/>
@@ -28146,8 +28216,9 @@
       <c r="BF58" s="74"/>
       <c r="BG58" s="74"/>
       <c r="BH58" s="74"/>
-    </row>
-    <row r="59" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI58" s="74"/>
+    </row>
+    <row r="59" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="74"/>
       <c r="B59" s="74"/>
       <c r="C59" s="22"/>
@@ -28167,10 +28238,10 @@
       <c r="Q59" s="74"/>
       <c r="R59" s="74"/>
       <c r="S59" s="74"/>
-      <c r="T59" s="23"/>
-      <c r="U59" s="74"/>
-      <c r="V59" s="23"/>
-      <c r="W59" s="74"/>
+      <c r="T59" s="74"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="74"/>
+      <c r="W59" s="23"/>
       <c r="X59" s="74"/>
       <c r="Y59" s="74"/>
       <c r="Z59" s="74"/>
@@ -28208,8 +28279,9 @@
       <c r="BF59" s="74"/>
       <c r="BG59" s="74"/>
       <c r="BH59" s="74"/>
-    </row>
-    <row r="60" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI59" s="74"/>
+    </row>
+    <row r="60" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="74"/>
       <c r="B60" s="74"/>
       <c r="C60" s="22"/>
@@ -28229,10 +28301,10 @@
       <c r="Q60" s="74"/>
       <c r="R60" s="74"/>
       <c r="S60" s="74"/>
-      <c r="T60" s="23"/>
-      <c r="U60" s="74"/>
-      <c r="V60" s="23"/>
-      <c r="W60" s="74"/>
+      <c r="T60" s="74"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="74"/>
+      <c r="W60" s="23"/>
       <c r="X60" s="74"/>
       <c r="Y60" s="74"/>
       <c r="Z60" s="74"/>
@@ -28270,8 +28342,9 @@
       <c r="BF60" s="74"/>
       <c r="BG60" s="74"/>
       <c r="BH60" s="74"/>
-    </row>
-    <row r="61" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI60" s="74"/>
+    </row>
+    <row r="61" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="74"/>
       <c r="B61" s="74"/>
       <c r="C61" s="22"/>
@@ -28291,10 +28364,10 @@
       <c r="Q61" s="74"/>
       <c r="R61" s="74"/>
       <c r="S61" s="74"/>
-      <c r="T61" s="23"/>
-      <c r="U61" s="74"/>
-      <c r="V61" s="23"/>
-      <c r="W61" s="74"/>
+      <c r="T61" s="74"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="74"/>
+      <c r="W61" s="23"/>
       <c r="X61" s="74"/>
       <c r="Y61" s="74"/>
       <c r="Z61" s="74"/>
@@ -28332,8 +28405,9 @@
       <c r="BF61" s="74"/>
       <c r="BG61" s="74"/>
       <c r="BH61" s="74"/>
-    </row>
-    <row r="62" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI61" s="74"/>
+    </row>
+    <row r="62" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="74"/>
       <c r="B62" s="74"/>
       <c r="C62" s="22"/>
@@ -28353,10 +28427,10 @@
       <c r="Q62" s="74"/>
       <c r="R62" s="74"/>
       <c r="S62" s="74"/>
-      <c r="T62" s="23"/>
-      <c r="U62" s="74"/>
-      <c r="V62" s="23"/>
-      <c r="W62" s="74"/>
+      <c r="T62" s="74"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="74"/>
+      <c r="W62" s="23"/>
       <c r="X62" s="74"/>
       <c r="Y62" s="74"/>
       <c r="Z62" s="74"/>
@@ -28394,8 +28468,9 @@
       <c r="BF62" s="74"/>
       <c r="BG62" s="74"/>
       <c r="BH62" s="74"/>
-    </row>
-    <row r="63" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI62" s="74"/>
+    </row>
+    <row r="63" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="74"/>
       <c r="B63" s="74"/>
       <c r="C63" s="22"/>
@@ -28415,10 +28490,10 @@
       <c r="Q63" s="74"/>
       <c r="R63" s="74"/>
       <c r="S63" s="74"/>
-      <c r="T63" s="23"/>
-      <c r="U63" s="74"/>
-      <c r="V63" s="23"/>
-      <c r="W63" s="74"/>
+      <c r="T63" s="74"/>
+      <c r="U63" s="23"/>
+      <c r="V63" s="74"/>
+      <c r="W63" s="23"/>
       <c r="X63" s="74"/>
       <c r="Y63" s="74"/>
       <c r="Z63" s="74"/>
@@ -28456,8 +28531,9 @@
       <c r="BF63" s="74"/>
       <c r="BG63" s="74"/>
       <c r="BH63" s="74"/>
-    </row>
-    <row r="64" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI63" s="74"/>
+    </row>
+    <row r="64" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="74"/>
       <c r="B64" s="74"/>
       <c r="C64" s="22"/>
@@ -28477,10 +28553,10 @@
       <c r="Q64" s="74"/>
       <c r="R64" s="74"/>
       <c r="S64" s="74"/>
-      <c r="T64" s="23"/>
-      <c r="U64" s="74"/>
-      <c r="V64" s="23"/>
-      <c r="W64" s="74"/>
+      <c r="T64" s="74"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="74"/>
+      <c r="W64" s="23"/>
       <c r="X64" s="74"/>
       <c r="Y64" s="74"/>
       <c r="Z64" s="74"/>
@@ -28518,8 +28594,9 @@
       <c r="BF64" s="74"/>
       <c r="BG64" s="74"/>
       <c r="BH64" s="74"/>
-    </row>
-    <row r="65" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI64" s="74"/>
+    </row>
+    <row r="65" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="74"/>
       <c r="B65" s="74"/>
       <c r="C65" s="22"/>
@@ -28539,10 +28616,10 @@
       <c r="Q65" s="74"/>
       <c r="R65" s="74"/>
       <c r="S65" s="74"/>
-      <c r="T65" s="23"/>
-      <c r="U65" s="74"/>
-      <c r="V65" s="23"/>
-      <c r="W65" s="74"/>
+      <c r="T65" s="74"/>
+      <c r="U65" s="23"/>
+      <c r="V65" s="74"/>
+      <c r="W65" s="23"/>
       <c r="X65" s="74"/>
       <c r="Y65" s="74"/>
       <c r="Z65" s="74"/>
@@ -28580,8 +28657,9 @@
       <c r="BF65" s="74"/>
       <c r="BG65" s="74"/>
       <c r="BH65" s="74"/>
-    </row>
-    <row r="66" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI65" s="74"/>
+    </row>
+    <row r="66" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="74"/>
       <c r="B66" s="74"/>
       <c r="C66" s="22"/>
@@ -28601,10 +28679,10 @@
       <c r="Q66" s="74"/>
       <c r="R66" s="74"/>
       <c r="S66" s="74"/>
-      <c r="T66" s="23"/>
-      <c r="U66" s="74"/>
-      <c r="V66" s="23"/>
-      <c r="W66" s="74"/>
+      <c r="T66" s="74"/>
+      <c r="U66" s="23"/>
+      <c r="V66" s="74"/>
+      <c r="W66" s="23"/>
       <c r="X66" s="74"/>
       <c r="Y66" s="74"/>
       <c r="Z66" s="74"/>
@@ -28642,8 +28720,9 @@
       <c r="BF66" s="74"/>
       <c r="BG66" s="74"/>
       <c r="BH66" s="74"/>
-    </row>
-    <row r="67" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI66" s="74"/>
+    </row>
+    <row r="67" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="74"/>
       <c r="B67" s="74"/>
       <c r="C67" s="22"/>
@@ -28663,10 +28742,10 @@
       <c r="Q67" s="74"/>
       <c r="R67" s="74"/>
       <c r="S67" s="74"/>
-      <c r="T67" s="23"/>
-      <c r="U67" s="74"/>
-      <c r="V67" s="23"/>
-      <c r="W67" s="74"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="74"/>
+      <c r="W67" s="23"/>
       <c r="X67" s="74"/>
       <c r="Y67" s="74"/>
       <c r="Z67" s="74"/>
@@ -28704,8 +28783,9 @@
       <c r="BF67" s="74"/>
       <c r="BG67" s="74"/>
       <c r="BH67" s="74"/>
-    </row>
-    <row r="68" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI67" s="74"/>
+    </row>
+    <row r="68" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="74"/>
       <c r="B68" s="74"/>
       <c r="C68" s="22"/>
@@ -28725,10 +28805,10 @@
       <c r="Q68" s="74"/>
       <c r="R68" s="74"/>
       <c r="S68" s="74"/>
-      <c r="T68" s="23"/>
-      <c r="U68" s="74"/>
-      <c r="V68" s="23"/>
-      <c r="W68" s="74"/>
+      <c r="T68" s="74"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="74"/>
+      <c r="W68" s="23"/>
       <c r="X68" s="74"/>
       <c r="Y68" s="74"/>
       <c r="Z68" s="74"/>
@@ -28766,8 +28846,9 @@
       <c r="BF68" s="74"/>
       <c r="BG68" s="74"/>
       <c r="BH68" s="74"/>
-    </row>
-    <row r="69" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI68" s="74"/>
+    </row>
+    <row r="69" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="74"/>
       <c r="B69" s="74"/>
       <c r="C69" s="22"/>
@@ -28787,10 +28868,10 @@
       <c r="Q69" s="74"/>
       <c r="R69" s="74"/>
       <c r="S69" s="74"/>
-      <c r="T69" s="23"/>
-      <c r="U69" s="74"/>
-      <c r="V69" s="23"/>
-      <c r="W69" s="74"/>
+      <c r="T69" s="74"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="74"/>
+      <c r="W69" s="23"/>
       <c r="X69" s="74"/>
       <c r="Y69" s="74"/>
       <c r="Z69" s="74"/>
@@ -28828,8 +28909,9 @@
       <c r="BF69" s="74"/>
       <c r="BG69" s="74"/>
       <c r="BH69" s="74"/>
-    </row>
-    <row r="70" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI69" s="74"/>
+    </row>
+    <row r="70" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="74"/>
       <c r="B70" s="74"/>
       <c r="C70" s="22"/>
@@ -28849,10 +28931,10 @@
       <c r="Q70" s="74"/>
       <c r="R70" s="74"/>
       <c r="S70" s="74"/>
-      <c r="T70" s="23"/>
-      <c r="U70" s="74"/>
-      <c r="V70" s="23"/>
-      <c r="W70" s="74"/>
+      <c r="T70" s="74"/>
+      <c r="U70" s="23"/>
+      <c r="V70" s="74"/>
+      <c r="W70" s="23"/>
       <c r="X70" s="74"/>
       <c r="Y70" s="74"/>
       <c r="Z70" s="74"/>
@@ -28890,8 +28972,9 @@
       <c r="BF70" s="74"/>
       <c r="BG70" s="74"/>
       <c r="BH70" s="74"/>
-    </row>
-    <row r="71" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI70" s="74"/>
+    </row>
+    <row r="71" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="74"/>
       <c r="B71" s="74"/>
       <c r="C71" s="22"/>
@@ -28911,10 +28994,10 @@
       <c r="Q71" s="74"/>
       <c r="R71" s="74"/>
       <c r="S71" s="74"/>
-      <c r="T71" s="23"/>
-      <c r="U71" s="74"/>
-      <c r="V71" s="23"/>
-      <c r="W71" s="74"/>
+      <c r="T71" s="74"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="74"/>
+      <c r="W71" s="23"/>
       <c r="X71" s="74"/>
       <c r="Y71" s="74"/>
       <c r="Z71" s="74"/>
@@ -28952,8 +29035,9 @@
       <c r="BF71" s="74"/>
       <c r="BG71" s="74"/>
       <c r="BH71" s="74"/>
-    </row>
-    <row r="72" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI71" s="74"/>
+    </row>
+    <row r="72" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="74"/>
       <c r="B72" s="74"/>
       <c r="C72" s="22"/>
@@ -28973,10 +29057,10 @@
       <c r="Q72" s="74"/>
       <c r="R72" s="74"/>
       <c r="S72" s="74"/>
-      <c r="T72" s="23"/>
-      <c r="U72" s="74"/>
-      <c r="V72" s="23"/>
-      <c r="W72" s="74"/>
+      <c r="T72" s="74"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="74"/>
+      <c r="W72" s="23"/>
       <c r="X72" s="74"/>
       <c r="Y72" s="74"/>
       <c r="Z72" s="74"/>
@@ -29014,8 +29098,9 @@
       <c r="BF72" s="74"/>
       <c r="BG72" s="74"/>
       <c r="BH72" s="74"/>
-    </row>
-    <row r="73" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI72" s="74"/>
+    </row>
+    <row r="73" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="74"/>
       <c r="B73" s="74"/>
       <c r="C73" s="22"/>
@@ -29035,10 +29120,10 @@
       <c r="Q73" s="74"/>
       <c r="R73" s="74"/>
       <c r="S73" s="74"/>
-      <c r="T73" s="23"/>
-      <c r="U73" s="74"/>
-      <c r="V73" s="23"/>
-      <c r="W73" s="74"/>
+      <c r="T73" s="74"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="74"/>
+      <c r="W73" s="23"/>
       <c r="X73" s="74"/>
       <c r="Y73" s="74"/>
       <c r="Z73" s="74"/>
@@ -29076,8 +29161,9 @@
       <c r="BF73" s="74"/>
       <c r="BG73" s="74"/>
       <c r="BH73" s="74"/>
-    </row>
-    <row r="74" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI73" s="74"/>
+    </row>
+    <row r="74" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="74"/>
       <c r="B74" s="74"/>
       <c r="C74" s="22"/>
@@ -29097,10 +29183,10 @@
       <c r="Q74" s="74"/>
       <c r="R74" s="74"/>
       <c r="S74" s="74"/>
-      <c r="T74" s="23"/>
-      <c r="U74" s="74"/>
-      <c r="V74" s="23"/>
-      <c r="W74" s="74"/>
+      <c r="T74" s="74"/>
+      <c r="U74" s="23"/>
+      <c r="V74" s="74"/>
+      <c r="W74" s="23"/>
       <c r="X74" s="74"/>
       <c r="Y74" s="74"/>
       <c r="Z74" s="74"/>
@@ -29138,8 +29224,9 @@
       <c r="BF74" s="74"/>
       <c r="BG74" s="74"/>
       <c r="BH74" s="74"/>
-    </row>
-    <row r="75" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI74" s="74"/>
+    </row>
+    <row r="75" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="74"/>
       <c r="B75" s="74"/>
       <c r="C75" s="22"/>
@@ -29159,10 +29246,10 @@
       <c r="Q75" s="74"/>
       <c r="R75" s="74"/>
       <c r="S75" s="74"/>
-      <c r="T75" s="23"/>
-      <c r="U75" s="74"/>
-      <c r="V75" s="23"/>
-      <c r="W75" s="74"/>
+      <c r="T75" s="74"/>
+      <c r="U75" s="23"/>
+      <c r="V75" s="74"/>
+      <c r="W75" s="23"/>
       <c r="X75" s="74"/>
       <c r="Y75" s="74"/>
       <c r="Z75" s="74"/>
@@ -29200,8 +29287,9 @@
       <c r="BF75" s="74"/>
       <c r="BG75" s="74"/>
       <c r="BH75" s="74"/>
-    </row>
-    <row r="76" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI75" s="74"/>
+    </row>
+    <row r="76" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="74"/>
       <c r="B76" s="74"/>
       <c r="C76" s="22"/>
@@ -29221,10 +29309,10 @@
       <c r="Q76" s="74"/>
       <c r="R76" s="74"/>
       <c r="S76" s="74"/>
-      <c r="T76" s="23"/>
-      <c r="U76" s="74"/>
-      <c r="V76" s="23"/>
-      <c r="W76" s="74"/>
+      <c r="T76" s="74"/>
+      <c r="U76" s="23"/>
+      <c r="V76" s="74"/>
+      <c r="W76" s="23"/>
       <c r="X76" s="74"/>
       <c r="Y76" s="74"/>
       <c r="Z76" s="74"/>
@@ -29262,8 +29350,9 @@
       <c r="BF76" s="74"/>
       <c r="BG76" s="74"/>
       <c r="BH76" s="74"/>
-    </row>
-    <row r="77" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI76" s="74"/>
+    </row>
+    <row r="77" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="74"/>
       <c r="B77" s="74"/>
       <c r="C77" s="22"/>
@@ -29283,10 +29372,10 @@
       <c r="Q77" s="74"/>
       <c r="R77" s="74"/>
       <c r="S77" s="74"/>
-      <c r="T77" s="23"/>
-      <c r="U77" s="74"/>
-      <c r="V77" s="23"/>
-      <c r="W77" s="74"/>
+      <c r="T77" s="74"/>
+      <c r="U77" s="23"/>
+      <c r="V77" s="74"/>
+      <c r="W77" s="23"/>
       <c r="X77" s="74"/>
       <c r="Y77" s="74"/>
       <c r="Z77" s="74"/>
@@ -29324,8 +29413,9 @@
       <c r="BF77" s="74"/>
       <c r="BG77" s="74"/>
       <c r="BH77" s="74"/>
-    </row>
-    <row r="78" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI77" s="74"/>
+    </row>
+    <row r="78" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="74"/>
       <c r="B78" s="74"/>
       <c r="C78" s="22"/>
@@ -29345,10 +29435,10 @@
       <c r="Q78" s="74"/>
       <c r="R78" s="74"/>
       <c r="S78" s="74"/>
-      <c r="T78" s="23"/>
-      <c r="U78" s="74"/>
-      <c r="V78" s="23"/>
-      <c r="W78" s="74"/>
+      <c r="T78" s="74"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="74"/>
+      <c r="W78" s="23"/>
       <c r="X78" s="74"/>
       <c r="Y78" s="74"/>
       <c r="Z78" s="74"/>
@@ -29386,8 +29476,9 @@
       <c r="BF78" s="74"/>
       <c r="BG78" s="74"/>
       <c r="BH78" s="74"/>
-    </row>
-    <row r="79" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI78" s="74"/>
+    </row>
+    <row r="79" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="74"/>
       <c r="B79" s="74"/>
       <c r="C79" s="22"/>
@@ -29407,10 +29498,10 @@
       <c r="Q79" s="74"/>
       <c r="R79" s="74"/>
       <c r="S79" s="74"/>
-      <c r="T79" s="23"/>
-      <c r="U79" s="74"/>
-      <c r="V79" s="23"/>
-      <c r="W79" s="74"/>
+      <c r="T79" s="74"/>
+      <c r="U79" s="23"/>
+      <c r="V79" s="74"/>
+      <c r="W79" s="23"/>
       <c r="X79" s="74"/>
       <c r="Y79" s="74"/>
       <c r="Z79" s="74"/>
@@ -29448,8 +29539,9 @@
       <c r="BF79" s="74"/>
       <c r="BG79" s="74"/>
       <c r="BH79" s="74"/>
-    </row>
-    <row r="80" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI79" s="74"/>
+    </row>
+    <row r="80" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="74"/>
       <c r="B80" s="74"/>
       <c r="C80" s="22"/>
@@ -29469,10 +29561,10 @@
       <c r="Q80" s="74"/>
       <c r="R80" s="74"/>
       <c r="S80" s="74"/>
-      <c r="T80" s="23"/>
-      <c r="U80" s="74"/>
-      <c r="V80" s="23"/>
-      <c r="W80" s="74"/>
+      <c r="T80" s="74"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="74"/>
+      <c r="W80" s="23"/>
       <c r="X80" s="74"/>
       <c r="Y80" s="74"/>
       <c r="Z80" s="74"/>
@@ -29510,8 +29602,9 @@
       <c r="BF80" s="74"/>
       <c r="BG80" s="74"/>
       <c r="BH80" s="74"/>
-    </row>
-    <row r="81" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI80" s="74"/>
+    </row>
+    <row r="81" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="74"/>
       <c r="B81" s="74"/>
       <c r="C81" s="22"/>
@@ -29531,10 +29624,10 @@
       <c r="Q81" s="74"/>
       <c r="R81" s="74"/>
       <c r="S81" s="74"/>
-      <c r="T81" s="23"/>
-      <c r="U81" s="74"/>
-      <c r="V81" s="23"/>
-      <c r="W81" s="74"/>
+      <c r="T81" s="74"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="74"/>
+      <c r="W81" s="23"/>
       <c r="X81" s="74"/>
       <c r="Y81" s="74"/>
       <c r="Z81" s="74"/>
@@ -29572,8 +29665,9 @@
       <c r="BF81" s="74"/>
       <c r="BG81" s="74"/>
       <c r="BH81" s="74"/>
-    </row>
-    <row r="82" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI81" s="74"/>
+    </row>
+    <row r="82" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="74"/>
       <c r="B82" s="74"/>
       <c r="C82" s="22"/>
@@ -29593,10 +29687,10 @@
       <c r="Q82" s="74"/>
       <c r="R82" s="74"/>
       <c r="S82" s="74"/>
-      <c r="T82" s="23"/>
-      <c r="U82" s="74"/>
-      <c r="V82" s="23"/>
-      <c r="W82" s="74"/>
+      <c r="T82" s="74"/>
+      <c r="U82" s="23"/>
+      <c r="V82" s="74"/>
+      <c r="W82" s="23"/>
       <c r="X82" s="74"/>
       <c r="Y82" s="74"/>
       <c r="Z82" s="74"/>
@@ -29634,8 +29728,9 @@
       <c r="BF82" s="74"/>
       <c r="BG82" s="74"/>
       <c r="BH82" s="74"/>
-    </row>
-    <row r="83" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI82" s="74"/>
+    </row>
+    <row r="83" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="74"/>
       <c r="B83" s="74"/>
       <c r="C83" s="22"/>
@@ -29655,10 +29750,10 @@
       <c r="Q83" s="74"/>
       <c r="R83" s="74"/>
       <c r="S83" s="74"/>
-      <c r="T83" s="23"/>
-      <c r="U83" s="74"/>
-      <c r="V83" s="23"/>
-      <c r="W83" s="74"/>
+      <c r="T83" s="74"/>
+      <c r="U83" s="23"/>
+      <c r="V83" s="74"/>
+      <c r="W83" s="23"/>
       <c r="X83" s="74"/>
       <c r="Y83" s="74"/>
       <c r="Z83" s="74"/>
@@ -29696,8 +29791,9 @@
       <c r="BF83" s="74"/>
       <c r="BG83" s="74"/>
       <c r="BH83" s="74"/>
-    </row>
-    <row r="84" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI83" s="74"/>
+    </row>
+    <row r="84" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="74"/>
       <c r="B84" s="74"/>
       <c r="C84" s="22"/>
@@ -29717,10 +29813,10 @@
       <c r="Q84" s="74"/>
       <c r="R84" s="74"/>
       <c r="S84" s="74"/>
-      <c r="T84" s="23"/>
-      <c r="U84" s="74"/>
-      <c r="V84" s="23"/>
-      <c r="W84" s="74"/>
+      <c r="T84" s="74"/>
+      <c r="U84" s="23"/>
+      <c r="V84" s="74"/>
+      <c r="W84" s="23"/>
       <c r="X84" s="74"/>
       <c r="Y84" s="74"/>
       <c r="Z84" s="74"/>
@@ -29758,8 +29854,9 @@
       <c r="BF84" s="74"/>
       <c r="BG84" s="74"/>
       <c r="BH84" s="74"/>
-    </row>
-    <row r="85" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI84" s="74"/>
+    </row>
+    <row r="85" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="74"/>
       <c r="B85" s="74"/>
       <c r="C85" s="22"/>
@@ -29779,10 +29876,10 @@
       <c r="Q85" s="74"/>
       <c r="R85" s="74"/>
       <c r="S85" s="74"/>
-      <c r="T85" s="23"/>
-      <c r="U85" s="74"/>
-      <c r="V85" s="23"/>
-      <c r="W85" s="74"/>
+      <c r="T85" s="74"/>
+      <c r="U85" s="23"/>
+      <c r="V85" s="74"/>
+      <c r="W85" s="23"/>
       <c r="X85" s="74"/>
       <c r="Y85" s="74"/>
       <c r="Z85" s="74"/>
@@ -29820,8 +29917,9 @@
       <c r="BF85" s="74"/>
       <c r="BG85" s="74"/>
       <c r="BH85" s="74"/>
-    </row>
-    <row r="86" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI85" s="74"/>
+    </row>
+    <row r="86" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="74"/>
       <c r="B86" s="74"/>
       <c r="C86" s="22"/>
@@ -29841,10 +29939,10 @@
       <c r="Q86" s="74"/>
       <c r="R86" s="74"/>
       <c r="S86" s="74"/>
-      <c r="T86" s="23"/>
-      <c r="U86" s="74"/>
-      <c r="V86" s="23"/>
-      <c r="W86" s="74"/>
+      <c r="T86" s="74"/>
+      <c r="U86" s="23"/>
+      <c r="V86" s="74"/>
+      <c r="W86" s="23"/>
       <c r="X86" s="74"/>
       <c r="Y86" s="74"/>
       <c r="Z86" s="74"/>
@@ -29882,8 +29980,9 @@
       <c r="BF86" s="74"/>
       <c r="BG86" s="74"/>
       <c r="BH86" s="74"/>
-    </row>
-    <row r="87" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI86" s="74"/>
+    </row>
+    <row r="87" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="74"/>
       <c r="B87" s="74"/>
       <c r="C87" s="22"/>
@@ -29903,10 +30002,10 @@
       <c r="Q87" s="74"/>
       <c r="R87" s="74"/>
       <c r="S87" s="74"/>
-      <c r="T87" s="23"/>
-      <c r="U87" s="74"/>
-      <c r="V87" s="23"/>
-      <c r="W87" s="74"/>
+      <c r="T87" s="74"/>
+      <c r="U87" s="23"/>
+      <c r="V87" s="74"/>
+      <c r="W87" s="23"/>
       <c r="X87" s="74"/>
       <c r="Y87" s="74"/>
       <c r="Z87" s="74"/>
@@ -29944,8 +30043,9 @@
       <c r="BF87" s="74"/>
       <c r="BG87" s="74"/>
       <c r="BH87" s="74"/>
-    </row>
-    <row r="88" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI87" s="74"/>
+    </row>
+    <row r="88" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="74"/>
       <c r="B88" s="74"/>
       <c r="C88" s="22"/>
@@ -30006,8 +30106,9 @@
       <c r="BF88" s="74"/>
       <c r="BG88" s="74"/>
       <c r="BH88" s="74"/>
-    </row>
-    <row r="89" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI88" s="74"/>
+    </row>
+    <row r="89" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="74"/>
       <c r="B89" s="74"/>
       <c r="C89" s="22"/>
@@ -30068,8 +30169,9 @@
       <c r="BF89" s="74"/>
       <c r="BG89" s="74"/>
       <c r="BH89" s="74"/>
-    </row>
-    <row r="90" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI89" s="74"/>
+    </row>
+    <row r="90" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="74"/>
       <c r="B90" s="74"/>
       <c r="C90" s="22"/>
@@ -30130,8 +30232,9 @@
       <c r="BF90" s="74"/>
       <c r="BG90" s="74"/>
       <c r="BH90" s="74"/>
-    </row>
-    <row r="91" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI90" s="74"/>
+    </row>
+    <row r="91" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="74"/>
       <c r="B91" s="74"/>
       <c r="C91" s="22"/>
@@ -30192,8 +30295,9 @@
       <c r="BF91" s="74"/>
       <c r="BG91" s="74"/>
       <c r="BH91" s="74"/>
-    </row>
-    <row r="92" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI91" s="74"/>
+    </row>
+    <row r="92" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="74"/>
       <c r="B92" s="74"/>
       <c r="C92" s="22"/>
@@ -30254,8 +30358,9 @@
       <c r="BF92" s="74"/>
       <c r="BG92" s="74"/>
       <c r="BH92" s="74"/>
-    </row>
-    <row r="93" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI92" s="74"/>
+    </row>
+    <row r="93" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="74"/>
       <c r="B93" s="74"/>
       <c r="C93" s="22"/>
@@ -30316,8 +30421,9 @@
       <c r="BF93" s="74"/>
       <c r="BG93" s="74"/>
       <c r="BH93" s="74"/>
-    </row>
-    <row r="94" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI93" s="74"/>
+    </row>
+    <row r="94" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="74"/>
       <c r="B94" s="74"/>
       <c r="C94" s="22"/>
@@ -30378,8 +30484,9 @@
       <c r="BF94" s="74"/>
       <c r="BG94" s="74"/>
       <c r="BH94" s="74"/>
-    </row>
-    <row r="95" spans="1:60" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI94" s="74"/>
+    </row>
+    <row r="95" spans="1:61" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="74"/>
       <c r="B95" s="74"/>
       <c r="C95" s="22"/>
@@ -30440,6 +30547,7 @@
       <c r="BF95" s="74"/>
       <c r="BG95" s="74"/>
       <c r="BH95" s="74"/>
+      <c r="BI95" s="74"/>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -30452,22 +30560,22 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E95" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R87" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S87" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Resident,Migratory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S87" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T87" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Rough guess (guesstimate),Ad hoc or opportunistic monitoring,Formal survey/census: total count (the total reserve sampled in an attempt to count all individuals present,e.g.,helicopter total count),Formal survey/census: total population estimated from s"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U87" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V87" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Aerial census - sample count (transects or blocks),Aerial census - total count – fixed wing,Aerial census – total count – helicopter,Call-up survey,Camera trap survey – with density estimation (e.g.,capture/recapture),Camera trap survey – without density"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W87" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X87" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Low/poor: only a small number of sample units (transects,camera traps,etc) that cover a small part of the reserve or are biased to certain areas,Medium/fair: sample units (transects,camera traps,etc) cover a fair proportion of the reserve and are fair"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2" xr:uid="{00000000-0002-0000-0200-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,2,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:X95" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y95" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>